<commit_message>
[Presentazione RQ] Inserita la presentazione
</commit_message>
<xml_diff>
--- a/RQ/Esterni/Piano di Progetto/Ripartizione ruoli e ore2.xlsx
+++ b/RQ/Esterni/Piano di Progetto/Ripartizione ruoli e ore2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="360" windowWidth="9645" windowHeight="4680" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="9645" windowHeight="4680" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prospetto orario (CON AN)" sheetId="2" r:id="rId1"/>
@@ -15,9 +15,6 @@
     <sheet name="4_VV" sheetId="5" r:id="rId6"/>
     <sheet name="Grafici" sheetId="8" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -1648,42 +1645,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1698,23 +1663,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2142,12 +2139,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="67953024"/>
-        <c:axId val="67954560"/>
+        <c:axId val="96412032"/>
+        <c:axId val="96413568"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="67953024"/>
+        <c:axId val="96412032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2156,7 +2153,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67954560"/>
+        <c:crossAx val="96413568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2164,7 +2161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="67954560"/>
+        <c:axId val="96413568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +2172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67953024"/>
+        <c:crossAx val="96412032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2365,12 +2362,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="69299584"/>
-        <c:axId val="69313664"/>
+        <c:axId val="96447872"/>
+        <c:axId val="96457856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="69299584"/>
+        <c:axId val="96447872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,7 +2376,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69313664"/>
+        <c:crossAx val="96457856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2387,7 +2384,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69313664"/>
+        <c:axId val="96457856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2399,7 +2396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69299584"/>
+        <c:crossAx val="96447872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2600,12 +2597,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="56305536"/>
-        <c:axId val="56307072"/>
+        <c:axId val="100936704"/>
+        <c:axId val="100954880"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="56305536"/>
+        <c:axId val="100936704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2614,7 +2611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56307072"/>
+        <c:crossAx val="100954880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2622,7 +2619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56307072"/>
+        <c:axId val="100954880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2634,7 +2631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56305536"/>
+        <c:crossAx val="100936704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2741,7 +2738,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Consuntivo_2_PA!$O$2:$O$6</c:f>
+              <c:f>'3_PDC'!$O$26:$O$30</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2751,13 +2748,13 @@
                   <c:v>Amministratore</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Analista</c:v>
+                  <c:v>Verificatore</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Verificatore</c:v>
+                  <c:v>Progettista</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Progettista</c:v>
+                  <c:v>Programmatore</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2805,7 +2802,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Consuntivo_2_PA!$O$2:$O$6</c:f>
+              <c:f>'3_PDC'!$O$26:$O$30</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2815,13 +2812,13 @@
                   <c:v>Amministratore</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Analista</c:v>
+                  <c:v>Verificatore</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Verificatore</c:v>
+                  <c:v>Progettista</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Progettista</c:v>
+                  <c:v>Programmatore</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2861,12 +2858,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="98534528"/>
-        <c:axId val="98536064"/>
+        <c:axId val="100968704"/>
+        <c:axId val="100974592"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98534528"/>
+        <c:axId val="100968704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2875,7 +2872,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98536064"/>
+        <c:crossAx val="100974592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2883,7 +2880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98536064"/>
+        <c:axId val="100974592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2891,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98534528"/>
+        <c:crossAx val="100968704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3419,11 +3416,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="85333504"/>
-        <c:axId val="85335040"/>
+        <c:axId val="101483264"/>
+        <c:axId val="101484800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85333504"/>
+        <c:axId val="101483264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3432,7 +3429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85335040"/>
+        <c:crossAx val="101484800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3440,7 +3437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85335040"/>
+        <c:axId val="101484800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3451,7 +3448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85333504"/>
+        <c:crossAx val="101483264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3927,42 +3924,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Prospetto orario (CON AN)"/>
-      <sheetName val="Prospetto orario (senza AN) (2)"/>
-      <sheetName val="1_AN"/>
-      <sheetName val="2_PA"/>
-      <sheetName val="3_PDC"/>
-      <sheetName val="4_VV"/>
-      <sheetName val="Grafici"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="7">
-          <cell r="Q7">
-            <v>4187</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="Q30">
-            <v>4217</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
@@ -4374,19 +4335,19 @@
         <f>'1_AN'!O2</f>
         <v>Membro</v>
       </c>
-      <c r="AC2" s="200" t="str">
+      <c r="AC2" s="205" t="str">
         <f>'1_AN'!P2</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD2" s="201"/>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="200" t="str">
+      <c r="AD2" s="206"/>
+      <c r="AE2" s="207"/>
+      <c r="AF2" s="205" t="str">
         <f>'1_AN'!S2</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG2" s="201"/>
-      <c r="AH2" s="201"/>
-      <c r="AI2" s="203" t="str">
+      <c r="AG2" s="206"/>
+      <c r="AH2" s="206"/>
+      <c r="AI2" s="199" t="str">
         <f>'1_AN'!V2</f>
         <v>Totale</v>
       </c>
@@ -4520,7 +4481,7 @@
         <f>'1_AN'!U3</f>
         <v>Fase</v>
       </c>
-      <c r="AI3" s="204"/>
+      <c r="AI3" s="200"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" s="139" t="s">
@@ -5403,25 +5364,25 @@
       <c r="AB12" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="AC12" s="200" t="str">
+      <c r="AC12" s="205" t="str">
         <f>Consuntivo_2_PA!V9</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD12" s="205"/>
-      <c r="AE12" s="206"/>
-      <c r="AF12" s="207" t="str">
+      <c r="AD12" s="208"/>
+      <c r="AE12" s="209"/>
+      <c r="AF12" s="195" t="str">
         <f>Consuntivo_2_PA!Y9</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG12" s="208"/>
-      <c r="AH12" s="209"/>
-      <c r="AI12" s="207" t="str">
+      <c r="AG12" s="196"/>
+      <c r="AH12" s="197"/>
+      <c r="AI12" s="195" t="str">
         <f>Consuntivo_2_PA!AB9</f>
         <v>III Periodo</v>
       </c>
-      <c r="AJ12" s="208"/>
-      <c r="AK12" s="210"/>
-      <c r="AL12" s="203" t="str">
+      <c r="AJ12" s="196"/>
+      <c r="AK12" s="198"/>
+      <c r="AL12" s="199" t="str">
         <f>Consuntivo_2_PA!AE9</f>
         <v>Totale</v>
       </c>
@@ -5472,7 +5433,7 @@
         <f>Consuntivo_2_PA!AD10</f>
         <v>Fase</v>
       </c>
-      <c r="AL13" s="204"/>
+      <c r="AL13" s="200"/>
       <c r="AM13" s="5">
         <f>SUM(AL14:AL27)</f>
         <v>193</v>
@@ -5527,7 +5488,7 @@
         <f>Consuntivo_2_PA!AD11</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL14" s="211">
+      <c r="AL14" s="201">
         <f>Consuntivo_2_PA!AE11</f>
         <v>26</v>
       </c>
@@ -5657,7 +5618,7 @@
         <f>Consuntivo_2_PA!AD12</f>
         <v>0</v>
       </c>
-      <c r="AL15" s="199"/>
+      <c r="AL15" s="193"/>
       <c r="AO15" s="5">
         <f>IF($AC15=AO$2,$AD15,0)</f>
         <v>0</v>
@@ -5776,7 +5737,7 @@
         <f>Consuntivo_2_PA!AD13</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL16" s="199">
+      <c r="AL16" s="193">
         <f>Consuntivo_2_PA!AE13</f>
         <v>27</v>
       </c>
@@ -5898,7 +5859,7 @@
         <f>Consuntivo_2_PA!AD14</f>
         <v>0</v>
       </c>
-      <c r="AL17" s="199"/>
+      <c r="AL17" s="193"/>
       <c r="AO17" s="5">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6017,7 +5978,7 @@
         <f>Consuntivo_2_PA!AD15</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL18" s="199">
+      <c r="AL18" s="193">
         <f>Consuntivo_2_PA!AE15</f>
         <v>26</v>
       </c>
@@ -6139,7 +6100,7 @@
         <f>Consuntivo_2_PA!AD16</f>
         <v>PA 6.1</v>
       </c>
-      <c r="AL19" s="199"/>
+      <c r="AL19" s="193"/>
       <c r="AO19" s="5">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6258,7 +6219,7 @@
         <f>Consuntivo_2_PA!AD17</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL20" s="199">
+      <c r="AL20" s="193">
         <f>Consuntivo_2_PA!AE17</f>
         <v>28</v>
       </c>
@@ -6380,7 +6341,7 @@
         <f>Consuntivo_2_PA!AD18</f>
         <v>PA 6.2</v>
       </c>
-      <c r="AL21" s="199"/>
+      <c r="AL21" s="193"/>
       <c r="AO21" s="5">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6499,7 +6460,7 @@
         <f>Consuntivo_2_PA!AD19</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL22" s="199">
+      <c r="AL22" s="193">
         <f>Consuntivo_2_PA!AE19</f>
         <v>30</v>
       </c>
@@ -6584,36 +6545,36 @@
       <c r="A23" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="212" t="s">
+      <c r="B23" s="210" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="212"/>
-      <c r="D23" s="212"/>
-      <c r="E23" s="212" t="s">
+      <c r="C23" s="210"/>
+      <c r="D23" s="210"/>
+      <c r="E23" s="210" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="212"/>
-      <c r="G23" s="212"/>
-      <c r="H23" s="212" t="s">
+      <c r="F23" s="210"/>
+      <c r="G23" s="210"/>
+      <c r="H23" s="210" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="212"/>
-      <c r="J23" s="212"/>
-      <c r="K23" s="212" t="s">
+      <c r="I23" s="210"/>
+      <c r="J23" s="210"/>
+      <c r="K23" s="210" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="212"/>
-      <c r="M23" s="212"/>
-      <c r="N23" s="212" t="s">
+      <c r="L23" s="210"/>
+      <c r="M23" s="210"/>
+      <c r="N23" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="O23" s="212"/>
-      <c r="P23" s="212"/>
-      <c r="Q23" s="212" t="s">
+      <c r="O23" s="210"/>
+      <c r="P23" s="210"/>
+      <c r="Q23" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="212"/>
-      <c r="S23" s="212"/>
+      <c r="R23" s="210"/>
+      <c r="S23" s="210"/>
       <c r="T23" s="150" t="s">
         <v>14</v>
       </c>
@@ -6658,7 +6619,7 @@
         <f>Consuntivo_2_PA!AD20</f>
         <v>0</v>
       </c>
-      <c r="AL23" s="199"/>
+      <c r="AL23" s="193"/>
       <c r="AO23" s="5">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -6737,50 +6698,50 @@
       </c>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A24" s="198" t="s">
+      <c r="A24" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="196">
+      <c r="B24" s="204">
         <f>SUM(AO4:AQ4,AO14:AQ15,AO31:AQ32,AO48:AQ49)</f>
         <v>17</v>
       </c>
-      <c r="C24" s="196"/>
-      <c r="D24" s="196"/>
-      <c r="E24" s="196">
+      <c r="C24" s="204"/>
+      <c r="D24" s="204"/>
+      <c r="E24" s="204">
         <f>SUM(AR4:AT4,AR14:AT15,AR31:AT32,AR48:AT49)</f>
         <v>10</v>
       </c>
-      <c r="F24" s="196"/>
-      <c r="G24" s="196"/>
-      <c r="H24" s="197">
+      <c r="F24" s="204"/>
+      <c r="G24" s="204"/>
+      <c r="H24" s="203">
         <f>SUM(AU4:AW4,AU14:AW15,AU31:AW32,AU48:AW49)</f>
         <v>15</v>
       </c>
-      <c r="I24" s="197"/>
-      <c r="J24" s="197"/>
-      <c r="K24" s="196">
+      <c r="I24" s="203"/>
+      <c r="J24" s="203"/>
+      <c r="K24" s="204">
         <f>SUM(AX4:AZ4,AX14:AZ15,AX31:AZ32,AX48:AZ49)</f>
         <v>10</v>
       </c>
-      <c r="L24" s="196"/>
-      <c r="M24" s="196"/>
-      <c r="N24" s="197">
+      <c r="L24" s="204"/>
+      <c r="M24" s="204"/>
+      <c r="N24" s="203">
         <f>SUM(BA4:BC4,BA14:BC15,BA31:BC32,BA48:BC49)</f>
         <v>59</v>
       </c>
-      <c r="O24" s="197"/>
-      <c r="P24" s="197"/>
-      <c r="Q24" s="196">
+      <c r="O24" s="203"/>
+      <c r="P24" s="203"/>
+      <c r="Q24" s="204">
         <f t="shared" ref="Q24" si="38">SUM(BD4:BF4,BD14:BF15,BD31:BF32,BD48:BF49)</f>
         <v>4</v>
       </c>
-      <c r="R24" s="196"/>
-      <c r="S24" s="196"/>
-      <c r="T24" s="194">
+      <c r="R24" s="204"/>
+      <c r="S24" s="204"/>
+      <c r="T24" s="213">
         <f t="shared" ref="T24" si="39">SUM(B24:S25)</f>
         <v>115</v>
       </c>
-      <c r="U24" s="193"/>
+      <c r="U24" s="212"/>
       <c r="AB24" s="44" t="str">
         <f>Consuntivo_2_PA!U21</f>
         <v>Quadrio Giacomo</v>
@@ -6821,7 +6782,7 @@
         <f>Consuntivo_2_PA!AD21</f>
         <v>PA 5.1, 6.2</v>
       </c>
-      <c r="AL24" s="199">
+      <c r="AL24" s="193">
         <f>Consuntivo_2_PA!AE21</f>
         <v>28</v>
       </c>
@@ -6903,27 +6864,27 @@
       </c>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A25" s="198"/>
-      <c r="B25" s="196"/>
-      <c r="C25" s="196"/>
-      <c r="D25" s="196"/>
-      <c r="E25" s="196"/>
-      <c r="F25" s="196"/>
-      <c r="G25" s="196"/>
-      <c r="H25" s="197"/>
-      <c r="I25" s="197"/>
-      <c r="J25" s="197"/>
-      <c r="K25" s="196"/>
-      <c r="L25" s="196"/>
-      <c r="M25" s="196"/>
-      <c r="N25" s="197"/>
-      <c r="O25" s="197"/>
-      <c r="P25" s="197"/>
-      <c r="Q25" s="196"/>
-      <c r="R25" s="196"/>
-      <c r="S25" s="196"/>
-      <c r="T25" s="194"/>
-      <c r="U25" s="193"/>
+      <c r="A25" s="202"/>
+      <c r="B25" s="204"/>
+      <c r="C25" s="204"/>
+      <c r="D25" s="204"/>
+      <c r="E25" s="204"/>
+      <c r="F25" s="204"/>
+      <c r="G25" s="204"/>
+      <c r="H25" s="203"/>
+      <c r="I25" s="203"/>
+      <c r="J25" s="203"/>
+      <c r="K25" s="204"/>
+      <c r="L25" s="204"/>
+      <c r="M25" s="204"/>
+      <c r="N25" s="203"/>
+      <c r="O25" s="203"/>
+      <c r="P25" s="203"/>
+      <c r="Q25" s="204"/>
+      <c r="R25" s="204"/>
+      <c r="S25" s="204"/>
+      <c r="T25" s="213"/>
+      <c r="U25" s="212"/>
       <c r="AB25" s="44">
         <f>Consuntivo_2_PA!U22</f>
         <v>0</v>
@@ -6964,7 +6925,7 @@
         <f>Consuntivo_2_PA!AD22</f>
         <v>0</v>
       </c>
-      <c r="AL25" s="199"/>
+      <c r="AL25" s="193"/>
       <c r="AO25" s="5">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -7043,50 +7004,50 @@
       </c>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A26" s="198" t="s">
+      <c r="A26" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="196">
+      <c r="B26" s="204">
         <f>SUM(AO5:AQ5,AO16:AQ17,AO33:AQ34,AO50:AQ51)</f>
         <v>13</v>
       </c>
-      <c r="C26" s="196"/>
-      <c r="D26" s="196"/>
-      <c r="E26" s="196">
+      <c r="C26" s="204"/>
+      <c r="D26" s="204"/>
+      <c r="E26" s="204">
         <f>SUM(AR5:AT5,AR16:AT17,AR33:AT34,AR50:AT51)</f>
         <v>10</v>
       </c>
-      <c r="F26" s="196"/>
-      <c r="G26" s="196"/>
-      <c r="H26" s="196">
+      <c r="F26" s="204"/>
+      <c r="G26" s="204"/>
+      <c r="H26" s="204">
         <f>SUM(AU5:AW5,AU16:AW17,AU33:AW34,AU50:AW51)</f>
         <v>11</v>
       </c>
-      <c r="I26" s="196"/>
-      <c r="J26" s="196"/>
-      <c r="K26" s="197">
+      <c r="I26" s="204"/>
+      <c r="J26" s="204"/>
+      <c r="K26" s="203">
         <f>SUM(AX5:AZ5,AX16:AZ17,AX33:AZ34,AX50:AZ51)</f>
         <v>41</v>
       </c>
-      <c r="L26" s="197"/>
-      <c r="M26" s="197"/>
-      <c r="N26" s="196">
+      <c r="L26" s="203"/>
+      <c r="M26" s="203"/>
+      <c r="N26" s="204">
         <f>SUM(BA5:BC5,BA16:BC17,BA33:BC34,BA50:BC51)</f>
         <v>29</v>
       </c>
-      <c r="O26" s="196"/>
-      <c r="P26" s="196"/>
-      <c r="Q26" s="196">
+      <c r="O26" s="204"/>
+      <c r="P26" s="204"/>
+      <c r="Q26" s="204">
         <f>SUM(BD5:BF5,BD16:BF17,BD33:BF34,BD50:BF51)</f>
         <v>12</v>
       </c>
-      <c r="R26" s="196"/>
-      <c r="S26" s="196"/>
-      <c r="T26" s="194">
+      <c r="R26" s="204"/>
+      <c r="S26" s="204"/>
+      <c r="T26" s="213">
         <f t="shared" ref="T26" si="40">SUM(B26:S27)</f>
         <v>116</v>
       </c>
-      <c r="U26" s="193"/>
+      <c r="U26" s="212"/>
       <c r="AB26" s="53" t="str">
         <f>Consuntivo_2_PA!U23</f>
         <v>Maggiolo Giorgio</v>
@@ -7127,7 +7088,7 @@
         <f>Consuntivo_2_PA!AD23</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL26" s="199">
+      <c r="AL26" s="193">
         <f>Consuntivo_2_PA!AE23</f>
         <v>28</v>
       </c>
@@ -7209,27 +7170,27 @@
       </c>
     </row>
     <row r="27" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="198"/>
-      <c r="B27" s="196"/>
-      <c r="C27" s="196"/>
-      <c r="D27" s="196"/>
-      <c r="E27" s="196"/>
-      <c r="F27" s="196"/>
-      <c r="G27" s="196"/>
-      <c r="H27" s="196"/>
-      <c r="I27" s="196"/>
-      <c r="J27" s="196"/>
-      <c r="K27" s="197"/>
-      <c r="L27" s="197"/>
-      <c r="M27" s="197"/>
-      <c r="N27" s="196"/>
-      <c r="O27" s="196"/>
-      <c r="P27" s="196"/>
-      <c r="Q27" s="196"/>
-      <c r="R27" s="196"/>
-      <c r="S27" s="196"/>
-      <c r="T27" s="194"/>
-      <c r="U27" s="193"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="204"/>
+      <c r="C27" s="204"/>
+      <c r="D27" s="204"/>
+      <c r="E27" s="204"/>
+      <c r="F27" s="204"/>
+      <c r="G27" s="204"/>
+      <c r="H27" s="204"/>
+      <c r="I27" s="204"/>
+      <c r="J27" s="204"/>
+      <c r="K27" s="203"/>
+      <c r="L27" s="203"/>
+      <c r="M27" s="203"/>
+      <c r="N27" s="204"/>
+      <c r="O27" s="204"/>
+      <c r="P27" s="204"/>
+      <c r="Q27" s="204"/>
+      <c r="R27" s="204"/>
+      <c r="S27" s="204"/>
+      <c r="T27" s="213"/>
+      <c r="U27" s="212"/>
       <c r="AB27" s="75">
         <f>Consuntivo_2_PA!U24</f>
         <v>0</v>
@@ -7270,7 +7231,7 @@
         <f>Consuntivo_2_PA!AD24</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL27" s="213"/>
+      <c r="AL27" s="194"/>
       <c r="AO27" s="5">
         <f t="shared" si="35"/>
         <v>0</v>
@@ -7349,96 +7310,96 @@
       </c>
     </row>
     <row r="28" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="198" t="s">
+      <c r="A28" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="196">
+      <c r="B28" s="204">
         <f>SUM(AO6:AQ6,AO18:AQ19,AO35:AQ36,AO52:AQ53)</f>
         <v>10</v>
       </c>
-      <c r="C28" s="196"/>
-      <c r="D28" s="196"/>
-      <c r="E28" s="196">
+      <c r="C28" s="204"/>
+      <c r="D28" s="204"/>
+      <c r="E28" s="204">
         <f>SUM(AR6:AT6,AR18:AT19,AR35:AT36,AR52:AT53)</f>
         <v>14</v>
       </c>
-      <c r="F28" s="196"/>
-      <c r="G28" s="196"/>
-      <c r="H28" s="196">
+      <c r="F28" s="204"/>
+      <c r="G28" s="204"/>
+      <c r="H28" s="204">
         <f>SUM(AU6:AW6,AU18:AW19,AU35:AW36,AU52:AW53)</f>
         <v>13</v>
       </c>
-      <c r="I28" s="196"/>
-      <c r="J28" s="196"/>
-      <c r="K28" s="196">
+      <c r="I28" s="204"/>
+      <c r="J28" s="204"/>
+      <c r="K28" s="204">
         <f>SUM(AX6:AZ6,AX18:AZ19,AX35:AZ36,AX52:AZ53)</f>
         <v>27</v>
       </c>
-      <c r="L28" s="196"/>
-      <c r="M28" s="196"/>
-      <c r="N28" s="196">
+      <c r="L28" s="204"/>
+      <c r="M28" s="204"/>
+      <c r="N28" s="204">
         <f>SUM(BA6:BC6,BA18:BC19,BA35:BC36,BA52:BC53)</f>
         <v>33</v>
       </c>
-      <c r="O28" s="196"/>
-      <c r="P28" s="196"/>
-      <c r="Q28" s="197">
+      <c r="O28" s="204"/>
+      <c r="P28" s="204"/>
+      <c r="Q28" s="203">
         <f>SUM(BD6:BF6,BD18:BF19,BD35:BF36,BD52:BF53)</f>
         <v>20</v>
       </c>
-      <c r="R28" s="197"/>
-      <c r="S28" s="197"/>
-      <c r="T28" s="194">
+      <c r="R28" s="203"/>
+      <c r="S28" s="203"/>
+      <c r="T28" s="213">
         <f t="shared" ref="T28" si="41">SUM(B28:S29)</f>
         <v>117</v>
       </c>
-      <c r="U28" s="193"/>
+      <c r="U28" s="212"/>
       <c r="BG28" s="144">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A29" s="198"/>
-      <c r="B29" s="196"/>
-      <c r="C29" s="196"/>
-      <c r="D29" s="196"/>
-      <c r="E29" s="196"/>
-      <c r="F29" s="196"/>
-      <c r="G29" s="196"/>
-      <c r="H29" s="196"/>
-      <c r="I29" s="196"/>
-      <c r="J29" s="196"/>
-      <c r="K29" s="196"/>
-      <c r="L29" s="196"/>
-      <c r="M29" s="196"/>
-      <c r="N29" s="196"/>
-      <c r="O29" s="196"/>
-      <c r="P29" s="196"/>
-      <c r="Q29" s="197"/>
-      <c r="R29" s="197"/>
-      <c r="S29" s="197"/>
-      <c r="T29" s="194"/>
-      <c r="U29" s="193"/>
+      <c r="A29" s="202"/>
+      <c r="B29" s="204"/>
+      <c r="C29" s="204"/>
+      <c r="D29" s="204"/>
+      <c r="E29" s="204"/>
+      <c r="F29" s="204"/>
+      <c r="G29" s="204"/>
+      <c r="H29" s="204"/>
+      <c r="I29" s="204"/>
+      <c r="J29" s="204"/>
+      <c r="K29" s="204"/>
+      <c r="L29" s="204"/>
+      <c r="M29" s="204"/>
+      <c r="N29" s="204"/>
+      <c r="O29" s="204"/>
+      <c r="P29" s="204"/>
+      <c r="Q29" s="203"/>
+      <c r="R29" s="203"/>
+      <c r="S29" s="203"/>
+      <c r="T29" s="213"/>
+      <c r="U29" s="212"/>
       <c r="AA29" s="5" t="s">
         <v>124</v>
       </c>
       <c r="AB29" s="140" t="s">
         <v>127</v>
       </c>
-      <c r="AC29" s="207" t="str">
+      <c r="AC29" s="195" t="str">
         <f>'3_PDC'!U6</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD29" s="208"/>
-      <c r="AE29" s="209"/>
-      <c r="AF29" s="207" t="str">
+      <c r="AD29" s="196"/>
+      <c r="AE29" s="197"/>
+      <c r="AF29" s="195" t="str">
         <f>'3_PDC'!X6</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG29" s="208"/>
-      <c r="AH29" s="210"/>
-      <c r="AI29" s="203" t="str">
+      <c r="AG29" s="196"/>
+      <c r="AH29" s="198"/>
+      <c r="AI29" s="199" t="str">
         <f>'3_PDC'!AA6</f>
         <v>Totale</v>
       </c>
@@ -7448,50 +7409,50 @@
       </c>
     </row>
     <row r="30" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="198" t="s">
+      <c r="A30" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="196">
+      <c r="B30" s="204">
         <f>SUM(AO7:AQ7,AO20:AQ21,AO37:AQ38,AO54:AQ55)</f>
         <v>15</v>
       </c>
-      <c r="C30" s="196"/>
-      <c r="D30" s="196"/>
-      <c r="E30" s="196">
+      <c r="C30" s="204"/>
+      <c r="D30" s="204"/>
+      <c r="E30" s="204">
         <f>SUM(AR7:AT7,AR20:AT21,AR37:AT38,AR54:AT55)</f>
         <v>4</v>
       </c>
-      <c r="F30" s="196"/>
-      <c r="G30" s="196"/>
-      <c r="H30" s="196">
+      <c r="F30" s="204"/>
+      <c r="G30" s="204"/>
+      <c r="H30" s="204">
         <f>SUM(AU7:AW7,AU20:AW21,AU37:AW38,AU54:AW55)</f>
         <v>11</v>
       </c>
-      <c r="I30" s="196"/>
-      <c r="J30" s="196"/>
-      <c r="K30" s="197">
+      <c r="I30" s="204"/>
+      <c r="J30" s="204"/>
+      <c r="K30" s="203">
         <f>SUM(AX7:AZ7,AX20:AZ21,AX37:AZ38,AX54:AZ55)</f>
         <v>39</v>
       </c>
-      <c r="L30" s="197"/>
-      <c r="M30" s="197"/>
-      <c r="N30" s="197">
+      <c r="L30" s="203"/>
+      <c r="M30" s="203"/>
+      <c r="N30" s="203">
         <f>SUM(BA7:BC7,BA20:BC21,BA37:BC38,BA54:BC55)</f>
         <v>35</v>
       </c>
-      <c r="O30" s="197"/>
-      <c r="P30" s="197"/>
-      <c r="Q30" s="196">
+      <c r="O30" s="203"/>
+      <c r="P30" s="203"/>
+      <c r="Q30" s="204">
         <f>SUM(BD7:BF7,BD20:BF21,BD37:BF38,BD54:BF55)</f>
         <v>18</v>
       </c>
-      <c r="R30" s="196"/>
-      <c r="S30" s="196"/>
-      <c r="T30" s="194">
+      <c r="R30" s="204"/>
+      <c r="S30" s="204"/>
+      <c r="T30" s="213">
         <f t="shared" ref="T30" si="42">SUM(B30:S31)</f>
         <v>122</v>
       </c>
-      <c r="U30" s="193"/>
+      <c r="U30" s="212"/>
       <c r="AB30" s="141"/>
       <c r="AC30" s="40" t="str">
         <f>'3_PDC'!U7</f>
@@ -7517,7 +7478,7 @@
         <f>'3_PDC'!Z7</f>
         <v>Fase</v>
       </c>
-      <c r="AI30" s="204"/>
+      <c r="AI30" s="200"/>
       <c r="AK30" s="5">
         <f>SUM(AI31:AI44)</f>
         <v>373</v>
@@ -7528,27 +7489,27 @@
       </c>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A31" s="198"/>
-      <c r="B31" s="196"/>
-      <c r="C31" s="196"/>
-      <c r="D31" s="196"/>
-      <c r="E31" s="196"/>
-      <c r="F31" s="196"/>
-      <c r="G31" s="196"/>
-      <c r="H31" s="196"/>
-      <c r="I31" s="196"/>
-      <c r="J31" s="196"/>
-      <c r="K31" s="197"/>
-      <c r="L31" s="197"/>
-      <c r="M31" s="197"/>
-      <c r="N31" s="197"/>
-      <c r="O31" s="197"/>
-      <c r="P31" s="197"/>
-      <c r="Q31" s="196"/>
-      <c r="R31" s="196"/>
-      <c r="S31" s="196"/>
-      <c r="T31" s="194"/>
-      <c r="U31" s="193"/>
+      <c r="A31" s="202"/>
+      <c r="B31" s="204"/>
+      <c r="C31" s="204"/>
+      <c r="D31" s="204"/>
+      <c r="E31" s="204"/>
+      <c r="F31" s="204"/>
+      <c r="G31" s="204"/>
+      <c r="H31" s="204"/>
+      <c r="I31" s="204"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="203"/>
+      <c r="L31" s="203"/>
+      <c r="M31" s="203"/>
+      <c r="N31" s="203"/>
+      <c r="O31" s="203"/>
+      <c r="P31" s="203"/>
+      <c r="Q31" s="204"/>
+      <c r="R31" s="204"/>
+      <c r="S31" s="204"/>
+      <c r="T31" s="213"/>
+      <c r="U31" s="212"/>
       <c r="AB31" s="44" t="str">
         <f>'3_PDC'!T8</f>
         <v>Begolo Marco</v>
@@ -7577,7 +7538,7 @@
         <f>'3_PDC'!Z8</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI31" s="211">
+      <c r="AI31" s="201">
         <f>'3_PDC'!AA8</f>
         <v>52</v>
       </c>
@@ -7663,50 +7624,50 @@
       </c>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A32" s="198" t="s">
+      <c r="A32" s="202" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="196">
+      <c r="B32" s="204">
         <f>SUM(AO8:AQ8,AO22:AQ23,AO39:AQ40,AO56:AQ57)</f>
         <v>9</v>
       </c>
-      <c r="C32" s="196"/>
-      <c r="D32" s="196"/>
-      <c r="E32" s="196">
+      <c r="C32" s="204"/>
+      <c r="D32" s="204"/>
+      <c r="E32" s="204">
         <f>SUM(AR8:AT8,AR22:AT23,AR39:AT40,AR56:AT57)</f>
         <v>11</v>
       </c>
-      <c r="F32" s="196"/>
-      <c r="G32" s="196"/>
-      <c r="H32" s="196">
+      <c r="F32" s="204"/>
+      <c r="G32" s="204"/>
+      <c r="H32" s="204">
         <f>SUM(AU8:AW8,AU22:AW23,AU39:AW40,AU56:AW57)</f>
         <v>12</v>
       </c>
-      <c r="I32" s="196"/>
-      <c r="J32" s="196"/>
-      <c r="K32" s="196">
+      <c r="I32" s="204"/>
+      <c r="J32" s="204"/>
+      <c r="K32" s="204">
         <f>SUM(AX8:AZ8,AX22:AZ23,AX39:AZ40,AX56:AZ57)</f>
         <v>30</v>
       </c>
-      <c r="L32" s="196"/>
-      <c r="M32" s="196"/>
-      <c r="N32" s="197">
+      <c r="L32" s="204"/>
+      <c r="M32" s="204"/>
+      <c r="N32" s="203">
         <f>SUM(BA8:BC8,BA22:BC23,BA39:BC40,BA56:BC57)</f>
         <v>37</v>
       </c>
-      <c r="O32" s="197"/>
-      <c r="P32" s="197"/>
-      <c r="Q32" s="196">
+      <c r="O32" s="203"/>
+      <c r="P32" s="203"/>
+      <c r="Q32" s="204">
         <f>SUM(BD8:BF8,BD22:BF23,BD39:BF40,BD56:BF57)</f>
         <v>23</v>
       </c>
-      <c r="R32" s="196"/>
-      <c r="S32" s="196"/>
-      <c r="T32" s="194">
+      <c r="R32" s="204"/>
+      <c r="S32" s="204"/>
+      <c r="T32" s="213">
         <f t="shared" ref="T32" si="58">SUM(B32:S33)</f>
         <v>122</v>
       </c>
-      <c r="U32" s="193"/>
+      <c r="U32" s="212"/>
       <c r="AB32" s="49">
         <f>'3_PDC'!T9</f>
         <v>0</v>
@@ -7735,7 +7696,7 @@
         <f>'3_PDC'!Z9</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI32" s="199"/>
+      <c r="AI32" s="193"/>
       <c r="AO32" s="5">
         <f>IF($AC32=AO$2,$AD32,0)</f>
         <v>0</v>
@@ -7814,27 +7775,27 @@
       </c>
     </row>
     <row r="33" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A33" s="198"/>
-      <c r="B33" s="196"/>
-      <c r="C33" s="196"/>
-      <c r="D33" s="196"/>
-      <c r="E33" s="196"/>
-      <c r="F33" s="196"/>
-      <c r="G33" s="196"/>
-      <c r="H33" s="196"/>
-      <c r="I33" s="196"/>
-      <c r="J33" s="196"/>
-      <c r="K33" s="196"/>
-      <c r="L33" s="196"/>
-      <c r="M33" s="196"/>
-      <c r="N33" s="197"/>
-      <c r="O33" s="197"/>
-      <c r="P33" s="197"/>
-      <c r="Q33" s="196"/>
-      <c r="R33" s="196"/>
-      <c r="S33" s="196"/>
-      <c r="T33" s="194"/>
-      <c r="U33" s="193"/>
+      <c r="A33" s="202"/>
+      <c r="B33" s="204"/>
+      <c r="C33" s="204"/>
+      <c r="D33" s="204"/>
+      <c r="E33" s="204"/>
+      <c r="F33" s="204"/>
+      <c r="G33" s="204"/>
+      <c r="H33" s="204"/>
+      <c r="I33" s="204"/>
+      <c r="J33" s="204"/>
+      <c r="K33" s="204"/>
+      <c r="L33" s="204"/>
+      <c r="M33" s="204"/>
+      <c r="N33" s="203"/>
+      <c r="O33" s="203"/>
+      <c r="P33" s="203"/>
+      <c r="Q33" s="204"/>
+      <c r="R33" s="204"/>
+      <c r="S33" s="204"/>
+      <c r="T33" s="213"/>
+      <c r="U33" s="212"/>
       <c r="AB33" s="44" t="str">
         <f>'3_PDC'!T10</f>
         <v>Facchin Gabriele</v>
@@ -7863,7 +7824,7 @@
         <f>'3_PDC'!Z10</f>
         <v>PDC 3.1</v>
       </c>
-      <c r="AI33" s="199">
+      <c r="AI33" s="193">
         <f>'3_PDC'!AA10</f>
         <v>52</v>
       </c>
@@ -7945,50 +7906,50 @@
       </c>
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A34" s="198" t="s">
+      <c r="A34" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="196">
+      <c r="B34" s="204">
         <f>SUM(AO9:AQ9,AO24:AQ25,AO41:AQ42,AO58:AQ59)</f>
         <v>6</v>
       </c>
-      <c r="C34" s="196"/>
-      <c r="D34" s="196"/>
-      <c r="E34" s="196">
+      <c r="C34" s="204"/>
+      <c r="D34" s="204"/>
+      <c r="E34" s="204">
         <f>SUM(AR9:AT9,AR24:AT25,AR41:AT42,AR58:AT59)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="196"/>
-      <c r="G34" s="196"/>
-      <c r="H34" s="196">
+      <c r="F34" s="204"/>
+      <c r="G34" s="204"/>
+      <c r="H34" s="204">
         <f>SUM(AU9:AW9,AU24:AW25,AU41:AW42,AU58:AW59)</f>
         <v>10</v>
       </c>
-      <c r="I34" s="196"/>
-      <c r="J34" s="196"/>
-      <c r="K34" s="197">
+      <c r="I34" s="204"/>
+      <c r="J34" s="204"/>
+      <c r="K34" s="203">
         <f>SUM(AX9:AZ9,AX24:AZ25,AX41:AZ42,AX58:AZ59)</f>
         <v>37</v>
       </c>
-      <c r="L34" s="197"/>
-      <c r="M34" s="197"/>
-      <c r="N34" s="197">
+      <c r="L34" s="203"/>
+      <c r="M34" s="203"/>
+      <c r="N34" s="203">
         <f>SUM(BA9:BC9,BA24:BC25,BA41:BC42,BA58:BC59)</f>
         <v>40</v>
       </c>
-      <c r="O34" s="197"/>
-      <c r="P34" s="197"/>
-      <c r="Q34" s="197">
+      <c r="O34" s="203"/>
+      <c r="P34" s="203"/>
+      <c r="Q34" s="203">
         <f>SUM(BD9:BF9,BD24:BF25,BD41:BF42,BD58:BF59)</f>
         <v>25</v>
       </c>
-      <c r="R34" s="197"/>
-      <c r="S34" s="197"/>
-      <c r="T34" s="194">
+      <c r="R34" s="203"/>
+      <c r="S34" s="203"/>
+      <c r="T34" s="213">
         <f t="shared" ref="T34" si="62">SUM(B34:S35)</f>
         <v>120</v>
       </c>
-      <c r="U34" s="193"/>
+      <c r="U34" s="212"/>
       <c r="AB34" s="44">
         <f>'3_PDC'!T11</f>
         <v>0</v>
@@ -8017,7 +7978,7 @@
         <f>'3_PDC'!Z11</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI34" s="199"/>
+      <c r="AI34" s="193"/>
       <c r="AO34" s="5">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8096,27 +8057,27 @@
       </c>
     </row>
     <row r="35" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A35" s="198"/>
-      <c r="B35" s="196"/>
-      <c r="C35" s="196"/>
-      <c r="D35" s="196"/>
-      <c r="E35" s="196"/>
-      <c r="F35" s="196"/>
-      <c r="G35" s="196"/>
-      <c r="H35" s="196"/>
-      <c r="I35" s="196"/>
-      <c r="J35" s="196"/>
-      <c r="K35" s="197"/>
-      <c r="L35" s="197"/>
-      <c r="M35" s="197"/>
-      <c r="N35" s="197"/>
-      <c r="O35" s="197"/>
-      <c r="P35" s="197"/>
-      <c r="Q35" s="197"/>
-      <c r="R35" s="197"/>
-      <c r="S35" s="197"/>
-      <c r="T35" s="194"/>
-      <c r="U35" s="193"/>
+      <c r="A35" s="202"/>
+      <c r="B35" s="204"/>
+      <c r="C35" s="204"/>
+      <c r="D35" s="204"/>
+      <c r="E35" s="204"/>
+      <c r="F35" s="204"/>
+      <c r="G35" s="204"/>
+      <c r="H35" s="204"/>
+      <c r="I35" s="204"/>
+      <c r="J35" s="204"/>
+      <c r="K35" s="203"/>
+      <c r="L35" s="203"/>
+      <c r="M35" s="203"/>
+      <c r="N35" s="203"/>
+      <c r="O35" s="203"/>
+      <c r="P35" s="203"/>
+      <c r="Q35" s="203"/>
+      <c r="R35" s="203"/>
+      <c r="S35" s="203"/>
+      <c r="T35" s="213"/>
+      <c r="U35" s="212"/>
       <c r="AB35" s="53" t="str">
         <f>'3_PDC'!T12</f>
         <v>Cornaglia Alessando</v>
@@ -8145,7 +8106,7 @@
         <f>'3_PDC'!Z12</f>
         <v>PDC 4.4 e 5</v>
       </c>
-      <c r="AI35" s="199">
+      <c r="AI35" s="193">
         <f>'3_PDC'!AA12</f>
         <v>52</v>
       </c>
@@ -8227,50 +8188,50 @@
       </c>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A36" s="198" t="s">
+      <c r="A36" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="196">
+      <c r="B36" s="204">
         <f>SUM(AO10:AQ10,AO26:AQ27,AO43:AQ44,AO60:AQ61)</f>
         <v>12</v>
       </c>
-      <c r="C36" s="196"/>
-      <c r="D36" s="196"/>
-      <c r="E36" s="196">
+      <c r="C36" s="204"/>
+      <c r="D36" s="204"/>
+      <c r="E36" s="204">
         <f>SUM(AR10:AT10,AR26:AT27,AR43:AT44,AR60:AT61)</f>
         <v>18</v>
       </c>
-      <c r="F36" s="196"/>
-      <c r="G36" s="196"/>
-      <c r="H36" s="196">
+      <c r="F36" s="204"/>
+      <c r="G36" s="204"/>
+      <c r="H36" s="204">
         <f>SUM(AU10:AW10,AU26:AW27,AU43:AW44,AU60:AW61)</f>
         <v>7</v>
       </c>
-      <c r="I36" s="196"/>
-      <c r="J36" s="196"/>
-      <c r="K36" s="197">
+      <c r="I36" s="204"/>
+      <c r="J36" s="204"/>
+      <c r="K36" s="203">
         <f>SUM(AX10:AZ10,AX26:AZ27,AX43:AZ44,AX60:AZ61)</f>
         <v>51</v>
       </c>
-      <c r="L36" s="197"/>
-      <c r="M36" s="197"/>
-      <c r="N36" s="196">
+      <c r="L36" s="203"/>
+      <c r="M36" s="203"/>
+      <c r="N36" s="204">
         <f>SUM(BA10:BC10,BA26:BC27,BA43:BC44,BA60:BC61)</f>
         <v>10</v>
       </c>
-      <c r="O36" s="196"/>
-      <c r="P36" s="196"/>
-      <c r="Q36" s="196">
+      <c r="O36" s="204"/>
+      <c r="P36" s="204"/>
+      <c r="Q36" s="204">
         <f>SUM(BD10:BF10,BD26:BF27,BD43:BF44,BD60:BF61)</f>
         <v>18</v>
       </c>
-      <c r="R36" s="196"/>
-      <c r="S36" s="196"/>
-      <c r="T36" s="194">
+      <c r="R36" s="204"/>
+      <c r="S36" s="204"/>
+      <c r="T36" s="213">
         <f t="shared" ref="T36" si="63">SUM(B36:S37)</f>
         <v>116</v>
       </c>
-      <c r="U36" s="193"/>
+      <c r="U36" s="212"/>
       <c r="AB36" s="49">
         <f>'3_PDC'!T13</f>
         <v>0</v>
@@ -8299,7 +8260,7 @@
         <f>'3_PDC'!Z13</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI36" s="199"/>
+      <c r="AI36" s="193"/>
       <c r="AO36" s="5">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8378,27 +8339,27 @@
       </c>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A37" s="198"/>
-      <c r="B37" s="196"/>
-      <c r="C37" s="196"/>
-      <c r="D37" s="196"/>
-      <c r="E37" s="196"/>
-      <c r="F37" s="196"/>
-      <c r="G37" s="196"/>
-      <c r="H37" s="196"/>
-      <c r="I37" s="196"/>
-      <c r="J37" s="196"/>
-      <c r="K37" s="197"/>
-      <c r="L37" s="197"/>
-      <c r="M37" s="197"/>
-      <c r="N37" s="196"/>
-      <c r="O37" s="196"/>
-      <c r="P37" s="196"/>
-      <c r="Q37" s="196"/>
-      <c r="R37" s="196"/>
-      <c r="S37" s="196"/>
-      <c r="T37" s="194"/>
-      <c r="U37" s="193"/>
+      <c r="A37" s="202"/>
+      <c r="B37" s="204"/>
+      <c r="C37" s="204"/>
+      <c r="D37" s="204"/>
+      <c r="E37" s="204"/>
+      <c r="F37" s="204"/>
+      <c r="G37" s="204"/>
+      <c r="H37" s="204"/>
+      <c r="I37" s="204"/>
+      <c r="J37" s="204"/>
+      <c r="K37" s="203"/>
+      <c r="L37" s="203"/>
+      <c r="M37" s="203"/>
+      <c r="N37" s="204"/>
+      <c r="O37" s="204"/>
+      <c r="P37" s="204"/>
+      <c r="Q37" s="204"/>
+      <c r="R37" s="204"/>
+      <c r="S37" s="204"/>
+      <c r="T37" s="213"/>
+      <c r="U37" s="212"/>
       <c r="AB37" s="44" t="str">
         <f>'3_PDC'!T14</f>
         <v>Dalla Pietà Massimo</v>
@@ -8427,7 +8388,7 @@
         <f>'3_PDC'!Z14</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI37" s="199">
+      <c r="AI37" s="193">
         <f>'3_PDC'!AA14</f>
         <v>57</v>
       </c>
@@ -8509,50 +8470,50 @@
       </c>
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A38" s="195" t="s">
+      <c r="A38" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="196">
+      <c r="B38" s="204">
         <f>SUM(B24:D37)</f>
         <v>82</v>
       </c>
-      <c r="C38" s="196"/>
-      <c r="D38" s="196"/>
-      <c r="E38" s="196">
+      <c r="C38" s="204"/>
+      <c r="D38" s="204"/>
+      <c r="E38" s="204">
         <f t="shared" ref="E38" si="64">SUM(E24:G37)</f>
         <v>69</v>
       </c>
-      <c r="F38" s="196"/>
-      <c r="G38" s="196"/>
-      <c r="H38" s="196">
+      <c r="F38" s="204"/>
+      <c r="G38" s="204"/>
+      <c r="H38" s="204">
         <f>SUM(H24:J37)</f>
         <v>79</v>
       </c>
-      <c r="I38" s="196"/>
-      <c r="J38" s="196"/>
-      <c r="K38" s="196">
+      <c r="I38" s="204"/>
+      <c r="J38" s="204"/>
+      <c r="K38" s="204">
         <f t="shared" ref="K38" si="65">SUM(K24:M37)</f>
         <v>235</v>
       </c>
-      <c r="L38" s="196"/>
-      <c r="M38" s="196"/>
-      <c r="N38" s="196">
+      <c r="L38" s="204"/>
+      <c r="M38" s="204"/>
+      <c r="N38" s="204">
         <f t="shared" ref="N38" si="66">SUM(N24:P37)</f>
         <v>243</v>
       </c>
-      <c r="O38" s="196"/>
-      <c r="P38" s="196"/>
-      <c r="Q38" s="196">
+      <c r="O38" s="204"/>
+      <c r="P38" s="204"/>
+      <c r="Q38" s="204">
         <f>SUM(Q24:S37)</f>
         <v>120</v>
       </c>
-      <c r="R38" s="196"/>
-      <c r="S38" s="196"/>
-      <c r="T38" s="194">
+      <c r="R38" s="204"/>
+      <c r="S38" s="204"/>
+      <c r="T38" s="213">
         <f>SUM(B38:S39)</f>
         <v>828</v>
       </c>
-      <c r="U38" s="193"/>
+      <c r="U38" s="212"/>
       <c r="AB38" s="44">
         <f>'3_PDC'!T15</f>
         <v>0</v>
@@ -8581,7 +8542,7 @@
         <f>'3_PDC'!Z15</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI38" s="199"/>
+      <c r="AI38" s="193"/>
       <c r="AO38" s="5">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8660,27 +8621,27 @@
       </c>
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A39" s="195"/>
-      <c r="B39" s="196"/>
-      <c r="C39" s="196"/>
-      <c r="D39" s="196"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="196"/>
-      <c r="H39" s="196"/>
-      <c r="I39" s="196"/>
-      <c r="J39" s="196"/>
-      <c r="K39" s="196"/>
-      <c r="L39" s="196"/>
-      <c r="M39" s="196"/>
-      <c r="N39" s="196"/>
-      <c r="O39" s="196"/>
-      <c r="P39" s="196"/>
-      <c r="Q39" s="196"/>
-      <c r="R39" s="196"/>
-      <c r="S39" s="196"/>
-      <c r="T39" s="194"/>
-      <c r="U39" s="193"/>
+      <c r="A39" s="211"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="204"/>
+      <c r="D39" s="204"/>
+      <c r="E39" s="204"/>
+      <c r="F39" s="204"/>
+      <c r="G39" s="204"/>
+      <c r="H39" s="204"/>
+      <c r="I39" s="204"/>
+      <c r="J39" s="204"/>
+      <c r="K39" s="204"/>
+      <c r="L39" s="204"/>
+      <c r="M39" s="204"/>
+      <c r="N39" s="204"/>
+      <c r="O39" s="204"/>
+      <c r="P39" s="204"/>
+      <c r="Q39" s="204"/>
+      <c r="R39" s="204"/>
+      <c r="S39" s="204"/>
+      <c r="T39" s="213"/>
+      <c r="U39" s="212"/>
       <c r="AB39" s="53" t="str">
         <f>'3_PDC'!T16</f>
         <v>Braghetto Lorenzo</v>
@@ -8709,7 +8670,7 @@
         <f>'3_PDC'!Z16</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI39" s="199">
+      <c r="AI39" s="193">
         <f>'3_PDC'!AA16</f>
         <v>54</v>
       </c>
@@ -8820,7 +8781,7 @@
         <f>'3_PDC'!Z17</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI40" s="199"/>
+      <c r="AI40" s="193"/>
       <c r="AO40" s="5">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -8928,7 +8889,7 @@
         <f>'3_PDC'!Z18</f>
         <v>PDC 6</v>
       </c>
-      <c r="AI41" s="199">
+      <c r="AI41" s="193">
         <f>'3_PDC'!AA18</f>
         <v>54</v>
       </c>
@@ -9039,7 +9000,7 @@
         <f>'3_PDC'!Z19</f>
         <v>PDC 3.2, 5 e 7</v>
       </c>
-      <c r="AI42" s="199"/>
+      <c r="AI42" s="193"/>
       <c r="AO42" s="5">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -9147,7 +9108,7 @@
         <f>'3_PDC'!Z20</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI43" s="199">
+      <c r="AI43" s="193">
         <f>'3_PDC'!AA20</f>
         <v>52</v>
       </c>
@@ -9258,7 +9219,7 @@
         <f>'3_PDC'!Z21</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI44" s="213"/>
+      <c r="AI44" s="194"/>
       <c r="AO44" s="5">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -9351,19 +9312,19 @@
       <c r="AB46" s="140" t="s">
         <v>128</v>
       </c>
-      <c r="AC46" s="207" t="str">
+      <c r="AC46" s="195" t="str">
         <f>'4_VV'!U3</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD46" s="208"/>
-      <c r="AE46" s="209"/>
-      <c r="AF46" s="207" t="str">
+      <c r="AD46" s="196"/>
+      <c r="AE46" s="197"/>
+      <c r="AF46" s="195" t="str">
         <f>'4_VV'!X3</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG46" s="208"/>
-      <c r="AH46" s="210"/>
-      <c r="AI46" s="203" t="str">
+      <c r="AG46" s="196"/>
+      <c r="AH46" s="198"/>
+      <c r="AI46" s="199" t="str">
         <f>'4_VV'!AA3</f>
         <v>Totale</v>
       </c>
@@ -9403,7 +9364,7 @@
         <f>'4_VV'!Z4</f>
         <v>Fase</v>
       </c>
-      <c r="AI47" s="204"/>
+      <c r="AI47" s="200"/>
       <c r="BG47" s="144">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -9439,7 +9400,7 @@
         <f>'4_VV'!Z5</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI48" s="211">
+      <c r="AI48" s="201">
         <f>'4_VV'!AA5</f>
         <v>18</v>
       </c>
@@ -9553,7 +9514,7 @@
         <f>'4_VV'!Z6</f>
         <v>0</v>
       </c>
-      <c r="AI49" s="199"/>
+      <c r="AI49" s="193"/>
       <c r="AO49" s="5">
         <f>IF($AC49=AO$2,$AD49,0)</f>
         <v>0</v>
@@ -9660,7 +9621,7 @@
         <f>'4_VV'!Z7</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI50" s="199">
+      <c r="AI50" s="193">
         <f>'4_VV'!AA7</f>
         <v>18</v>
       </c>
@@ -9782,7 +9743,7 @@
         <f>'4_VV'!Z8</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI51" s="199"/>
+      <c r="AI51" s="193"/>
       <c r="AO51" s="5">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -9903,7 +9864,7 @@
         <f>'4_VV'!Z9</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI52" s="199">
+      <c r="AI52" s="193">
         <f>'4_VV'!AA9</f>
         <v>18</v>
       </c>
@@ -10027,7 +9988,7 @@
         <f>'4_VV'!Z10</f>
         <v>0</v>
       </c>
-      <c r="AI53" s="199"/>
+      <c r="AI53" s="193"/>
       <c r="AO53" s="5">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -10148,7 +10109,7 @@
         <f>'4_VV'!Z11</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI54" s="199">
+      <c r="AI54" s="193">
         <f>'4_VV'!AA11</f>
         <v>18</v>
       </c>
@@ -10272,7 +10233,7 @@
         <f>'4_VV'!Z12</f>
         <v>0</v>
       </c>
-      <c r="AI55" s="199"/>
+      <c r="AI55" s="193"/>
       <c r="AO55" s="5">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -10393,7 +10354,7 @@
         <f>'4_VV'!Z13</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI56" s="199">
+      <c r="AI56" s="193">
         <f>'4_VV'!AA13</f>
         <v>18</v>
       </c>
@@ -10517,7 +10478,7 @@
         <f>'4_VV'!Z14</f>
         <v>0</v>
       </c>
-      <c r="AI57" s="199"/>
+      <c r="AI57" s="193"/>
       <c r="AO57" s="5">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -10635,7 +10596,7 @@
         <f>'4_VV'!Z15</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI58" s="199">
+      <c r="AI58" s="193">
         <f>'4_VV'!AA15</f>
         <v>18</v>
       </c>
@@ -10745,7 +10706,7 @@
         <f>'4_VV'!Z16</f>
         <v>0</v>
       </c>
-      <c r="AI59" s="199"/>
+      <c r="AI59" s="193"/>
       <c r="AO59" s="5">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -10852,7 +10813,7 @@
         <f>'4_VV'!Z17</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI60" s="199">
+      <c r="AI60" s="193">
         <f>'4_VV'!AA17</f>
         <v>16</v>
       </c>
@@ -10962,7 +10923,7 @@
         <f>'4_VV'!Z18</f>
         <v>0</v>
       </c>
-      <c r="AI61" s="213"/>
+      <c r="AI61" s="194"/>
       <c r="AO61" s="5">
         <f t="shared" si="82"/>
         <v>0</v>
@@ -11042,78 +11003,22 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="AI43:AI44"/>
-    <mergeCell ref="AC46:AE46"/>
-    <mergeCell ref="AF46:AH46"/>
-    <mergeCell ref="AI46:AI47"/>
-    <mergeCell ref="AI60:AI61"/>
-    <mergeCell ref="AI48:AI49"/>
-    <mergeCell ref="AI50:AI51"/>
-    <mergeCell ref="AI52:AI53"/>
-    <mergeCell ref="AI54:AI55"/>
-    <mergeCell ref="AI56:AI57"/>
-    <mergeCell ref="AI58:AI59"/>
-    <mergeCell ref="AI41:AI42"/>
-    <mergeCell ref="AL24:AL25"/>
-    <mergeCell ref="AL26:AL27"/>
-    <mergeCell ref="AC29:AE29"/>
-    <mergeCell ref="AF29:AH29"/>
-    <mergeCell ref="AI29:AI30"/>
-    <mergeCell ref="AI31:AI32"/>
-    <mergeCell ref="AI33:AI34"/>
-    <mergeCell ref="AI35:AI36"/>
-    <mergeCell ref="AI37:AI38"/>
-    <mergeCell ref="AI39:AI40"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="H24:J25"/>
-    <mergeCell ref="E24:G25"/>
-    <mergeCell ref="B24:D25"/>
-    <mergeCell ref="AL22:AL23"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC12:AE12"/>
-    <mergeCell ref="AF12:AH12"/>
-    <mergeCell ref="AI12:AK12"/>
-    <mergeCell ref="AL12:AL13"/>
-    <mergeCell ref="AL14:AL15"/>
-    <mergeCell ref="AL16:AL17"/>
-    <mergeCell ref="AL18:AL19"/>
-    <mergeCell ref="AL20:AL21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="Q23:S23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:D27"/>
-    <mergeCell ref="E26:G27"/>
-    <mergeCell ref="H26:J27"/>
-    <mergeCell ref="K26:M27"/>
-    <mergeCell ref="E30:G31"/>
-    <mergeCell ref="H30:J31"/>
-    <mergeCell ref="K30:M31"/>
-    <mergeCell ref="N26:P27"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="K32:M33"/>
-    <mergeCell ref="N32:P33"/>
-    <mergeCell ref="Q32:S33"/>
-    <mergeCell ref="Q24:S25"/>
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="K24:M25"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="Q26:S27"/>
-    <mergeCell ref="K28:M29"/>
-    <mergeCell ref="N28:P29"/>
-    <mergeCell ref="Q28:S29"/>
-    <mergeCell ref="B30:D31"/>
-    <mergeCell ref="B28:D29"/>
-    <mergeCell ref="E28:G29"/>
-    <mergeCell ref="H28:J29"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="U24:U25"/>
+    <mergeCell ref="U36:U37"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="T36:T37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:D39"/>
     <mergeCell ref="E38:G39"/>
@@ -11138,22 +11043,78 @@
     <mergeCell ref="N36:P37"/>
     <mergeCell ref="Q36:S37"/>
     <mergeCell ref="Q34:S35"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="U24:U25"/>
-    <mergeCell ref="U36:U37"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="T32:T33"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="T36:T37"/>
+    <mergeCell ref="K32:M33"/>
+    <mergeCell ref="N32:P33"/>
+    <mergeCell ref="Q32:S33"/>
+    <mergeCell ref="Q24:S25"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="K24:M25"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="Q26:S27"/>
+    <mergeCell ref="K28:M29"/>
+    <mergeCell ref="N28:P29"/>
+    <mergeCell ref="Q28:S29"/>
+    <mergeCell ref="B30:D31"/>
+    <mergeCell ref="B28:D29"/>
+    <mergeCell ref="E28:G29"/>
+    <mergeCell ref="H28:J29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:D27"/>
+    <mergeCell ref="E26:G27"/>
+    <mergeCell ref="H26:J27"/>
+    <mergeCell ref="K26:M27"/>
+    <mergeCell ref="E30:G31"/>
+    <mergeCell ref="H30:J31"/>
+    <mergeCell ref="K30:M31"/>
+    <mergeCell ref="N26:P27"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="H24:J25"/>
+    <mergeCell ref="E24:G25"/>
+    <mergeCell ref="B24:D25"/>
+    <mergeCell ref="AL22:AL23"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AC12:AE12"/>
+    <mergeCell ref="AF12:AH12"/>
+    <mergeCell ref="AI12:AK12"/>
+    <mergeCell ref="AL12:AL13"/>
+    <mergeCell ref="AL14:AL15"/>
+    <mergeCell ref="AL16:AL17"/>
+    <mergeCell ref="AL18:AL19"/>
+    <mergeCell ref="AL20:AL21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="AI41:AI42"/>
+    <mergeCell ref="AL24:AL25"/>
+    <mergeCell ref="AL26:AL27"/>
+    <mergeCell ref="AC29:AE29"/>
+    <mergeCell ref="AF29:AH29"/>
+    <mergeCell ref="AI29:AI30"/>
+    <mergeCell ref="AI31:AI32"/>
+    <mergeCell ref="AI33:AI34"/>
+    <mergeCell ref="AI35:AI36"/>
+    <mergeCell ref="AI37:AI38"/>
+    <mergeCell ref="AI39:AI40"/>
+    <mergeCell ref="AI43:AI44"/>
+    <mergeCell ref="AC46:AE46"/>
+    <mergeCell ref="AF46:AH46"/>
+    <mergeCell ref="AI46:AI47"/>
+    <mergeCell ref="AI60:AI61"/>
+    <mergeCell ref="AI48:AI49"/>
+    <mergeCell ref="AI50:AI51"/>
+    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="AI54:AI55"/>
+    <mergeCell ref="AI56:AI57"/>
+    <mergeCell ref="AI58:AI59"/>
   </mergeCells>
   <conditionalFormatting sqref="AB14:AL27">
     <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
@@ -11267,13 +11228,13 @@
         <v>74</v>
       </c>
       <c r="AB2" s="140"/>
-      <c r="AC2" s="200"/>
-      <c r="AD2" s="201"/>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="200"/>
-      <c r="AG2" s="201"/>
-      <c r="AH2" s="201"/>
-      <c r="AI2" s="203"/>
+      <c r="AC2" s="205"/>
+      <c r="AD2" s="206"/>
+      <c r="AE2" s="207"/>
+      <c r="AF2" s="205"/>
+      <c r="AG2" s="206"/>
+      <c r="AH2" s="206"/>
+      <c r="AI2" s="199"/>
       <c r="AJ2" s="5">
         <f>SUM(AI4:AI10)</f>
         <v>0</v>
@@ -11363,7 +11324,7 @@
       <c r="AF3" s="87"/>
       <c r="AG3" s="88"/>
       <c r="AH3" s="142"/>
-      <c r="AI3" s="204"/>
+      <c r="AI3" s="200"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" s="139"/>
@@ -11976,25 +11937,25 @@
       <c r="AB12" s="140" t="s">
         <v>126</v>
       </c>
-      <c r="AC12" s="200" t="str">
+      <c r="AC12" s="205" t="str">
         <f>Consuntivo_2_PA!V9</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD12" s="205"/>
-      <c r="AE12" s="206"/>
-      <c r="AF12" s="207" t="str">
+      <c r="AD12" s="208"/>
+      <c r="AE12" s="209"/>
+      <c r="AF12" s="195" t="str">
         <f>Consuntivo_2_PA!Y9</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG12" s="208"/>
-      <c r="AH12" s="209"/>
-      <c r="AI12" s="207" t="str">
+      <c r="AG12" s="196"/>
+      <c r="AH12" s="197"/>
+      <c r="AI12" s="195" t="str">
         <f>Consuntivo_2_PA!AB9</f>
         <v>III Periodo</v>
       </c>
-      <c r="AJ12" s="208"/>
-      <c r="AK12" s="210"/>
-      <c r="AL12" s="203" t="str">
+      <c r="AJ12" s="196"/>
+      <c r="AK12" s="198"/>
+      <c r="AL12" s="199" t="str">
         <f>Consuntivo_2_PA!AE9</f>
         <v>Totale</v>
       </c>
@@ -12041,7 +12002,7 @@
         <f>Consuntivo_2_PA!AD10</f>
         <v>Fase</v>
       </c>
-      <c r="AL13" s="204"/>
+      <c r="AL13" s="200"/>
       <c r="AM13" s="5">
         <f>SUM(AL14:AL27)</f>
         <v>193</v>
@@ -12092,7 +12053,7 @@
         <f>Consuntivo_2_PA!AD11</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL14" s="211">
+      <c r="AL14" s="201">
         <f>Consuntivo_2_PA!AE11</f>
         <v>26</v>
       </c>
@@ -12218,7 +12179,7 @@
         <f>Consuntivo_2_PA!AD12</f>
         <v>0</v>
       </c>
-      <c r="AL15" s="199"/>
+      <c r="AL15" s="193"/>
       <c r="AO15" s="5">
         <f>IF($AC15=AO$2,$AD15,0)</f>
         <v>0</v>
@@ -12337,7 +12298,7 @@
         <f>Consuntivo_2_PA!AD13</f>
         <v>PA 3.2</v>
       </c>
-      <c r="AL16" s="199">
+      <c r="AL16" s="193">
         <f>Consuntivo_2_PA!AE13</f>
         <v>27</v>
       </c>
@@ -12459,7 +12420,7 @@
         <f>Consuntivo_2_PA!AD14</f>
         <v>0</v>
       </c>
-      <c r="AL17" s="199"/>
+      <c r="AL17" s="193"/>
       <c r="AO17" s="5">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -12578,7 +12539,7 @@
         <f>Consuntivo_2_PA!AD15</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL18" s="199">
+      <c r="AL18" s="193">
         <f>Consuntivo_2_PA!AE15</f>
         <v>26</v>
       </c>
@@ -12700,7 +12661,7 @@
         <f>Consuntivo_2_PA!AD16</f>
         <v>PA 6.1</v>
       </c>
-      <c r="AL19" s="199"/>
+      <c r="AL19" s="193"/>
       <c r="AO19" s="5">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -12819,7 +12780,7 @@
         <f>Consuntivo_2_PA!AD17</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL20" s="199">
+      <c r="AL20" s="193">
         <f>Consuntivo_2_PA!AE17</f>
         <v>28</v>
       </c>
@@ -12941,7 +12902,7 @@
         <f>Consuntivo_2_PA!AD18</f>
         <v>PA 6.2</v>
       </c>
-      <c r="AL21" s="199"/>
+      <c r="AL21" s="193"/>
       <c r="AO21" s="5">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -13060,7 +13021,7 @@
         <f>Consuntivo_2_PA!AD19</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL22" s="199">
+      <c r="AL22" s="193">
         <f>Consuntivo_2_PA!AE19</f>
         <v>30</v>
       </c>
@@ -13145,36 +13106,36 @@
       <c r="A23" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="212" t="s">
+      <c r="B23" s="210" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="212"/>
-      <c r="D23" s="212"/>
-      <c r="E23" s="212" t="s">
+      <c r="C23" s="210"/>
+      <c r="D23" s="210"/>
+      <c r="E23" s="210" t="s">
         <v>2</v>
       </c>
-      <c r="F23" s="212"/>
-      <c r="G23" s="212"/>
-      <c r="H23" s="212" t="s">
+      <c r="F23" s="210"/>
+      <c r="G23" s="210"/>
+      <c r="H23" s="210" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="212"/>
-      <c r="J23" s="212"/>
-      <c r="K23" s="212" t="s">
+      <c r="I23" s="210"/>
+      <c r="J23" s="210"/>
+      <c r="K23" s="210" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="212"/>
-      <c r="M23" s="212"/>
-      <c r="N23" s="212" t="s">
+      <c r="L23" s="210"/>
+      <c r="M23" s="210"/>
+      <c r="N23" s="210" t="s">
         <v>5</v>
       </c>
-      <c r="O23" s="212"/>
-      <c r="P23" s="212"/>
-      <c r="Q23" s="212" t="s">
+      <c r="O23" s="210"/>
+      <c r="P23" s="210"/>
+      <c r="Q23" s="210" t="s">
         <v>6</v>
       </c>
-      <c r="R23" s="212"/>
-      <c r="S23" s="212"/>
+      <c r="R23" s="210"/>
+      <c r="S23" s="210"/>
       <c r="T23" s="149" t="s">
         <v>14</v>
       </c>
@@ -13219,7 +13180,7 @@
         <f>Consuntivo_2_PA!AD20</f>
         <v>0</v>
       </c>
-      <c r="AL23" s="199"/>
+      <c r="AL23" s="193"/>
       <c r="AO23" s="5">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -13298,50 +13259,50 @@
       </c>
     </row>
     <row r="24" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A24" s="198" t="s">
+      <c r="A24" s="202" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="196">
+      <c r="B24" s="204">
         <f>SUM(AO4:AQ4,AO14:AQ15,AO31:AQ32,AO48:AQ49)</f>
         <v>4</v>
       </c>
-      <c r="C24" s="196"/>
-      <c r="D24" s="196"/>
-      <c r="E24" s="196">
+      <c r="C24" s="204"/>
+      <c r="D24" s="204"/>
+      <c r="E24" s="204">
         <f>SUM(AR4:AT4,AR14:AT15,AR31:AT32,AR48:AT49)</f>
         <v>10</v>
       </c>
-      <c r="F24" s="196"/>
-      <c r="G24" s="196"/>
-      <c r="H24" s="197">
+      <c r="F24" s="204"/>
+      <c r="G24" s="204"/>
+      <c r="H24" s="203">
         <f>SUM(AU4:AW4,AU14:AW15,AU31:AW32,AU48:AW49)</f>
         <v>9</v>
       </c>
-      <c r="I24" s="197"/>
-      <c r="J24" s="197"/>
-      <c r="K24" s="196">
+      <c r="I24" s="203"/>
+      <c r="J24" s="203"/>
+      <c r="K24" s="204">
         <f>SUM(AX4:AZ4,AX14:AZ15,AX31:AZ32,AX48:AZ49)</f>
         <v>10</v>
       </c>
-      <c r="L24" s="196"/>
-      <c r="M24" s="196"/>
-      <c r="N24" s="197">
+      <c r="L24" s="204"/>
+      <c r="M24" s="204"/>
+      <c r="N24" s="203">
         <f>SUM(BA4:BC4,BA14:BC15,BA31:BC32,BA48:BC49)</f>
         <v>59</v>
       </c>
-      <c r="O24" s="197"/>
-      <c r="P24" s="197"/>
-      <c r="Q24" s="196">
+      <c r="O24" s="203"/>
+      <c r="P24" s="203"/>
+      <c r="Q24" s="204">
         <f>SUM(BD4:BF4,BD14:BF15,BD31:BF32,BD48:BF49)</f>
         <v>4</v>
       </c>
-      <c r="R24" s="196"/>
-      <c r="S24" s="196"/>
-      <c r="T24" s="196">
+      <c r="R24" s="204"/>
+      <c r="S24" s="204"/>
+      <c r="T24" s="204">
         <f t="shared" ref="T24" si="32">SUM(B24:S25)</f>
         <v>96</v>
       </c>
-      <c r="U24" s="193"/>
+      <c r="U24" s="212"/>
       <c r="AB24" s="44" t="str">
         <f>Consuntivo_2_PA!U21</f>
         <v>Quadrio Giacomo</v>
@@ -13382,7 +13343,7 @@
         <f>Consuntivo_2_PA!AD21</f>
         <v>PA 5.1, 6.2</v>
       </c>
-      <c r="AL24" s="199">
+      <c r="AL24" s="193">
         <f>Consuntivo_2_PA!AE21</f>
         <v>28</v>
       </c>
@@ -13464,27 +13425,27 @@
       </c>
     </row>
     <row r="25" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A25" s="198"/>
-      <c r="B25" s="196"/>
-      <c r="C25" s="196"/>
-      <c r="D25" s="196"/>
-      <c r="E25" s="196"/>
-      <c r="F25" s="196"/>
-      <c r="G25" s="196"/>
-      <c r="H25" s="197"/>
-      <c r="I25" s="197"/>
-      <c r="J25" s="197"/>
-      <c r="K25" s="196"/>
-      <c r="L25" s="196"/>
-      <c r="M25" s="196"/>
-      <c r="N25" s="197"/>
-      <c r="O25" s="197"/>
-      <c r="P25" s="197"/>
-      <c r="Q25" s="196"/>
-      <c r="R25" s="196"/>
-      <c r="S25" s="196"/>
-      <c r="T25" s="196"/>
-      <c r="U25" s="193"/>
+      <c r="A25" s="202"/>
+      <c r="B25" s="204"/>
+      <c r="C25" s="204"/>
+      <c r="D25" s="204"/>
+      <c r="E25" s="204"/>
+      <c r="F25" s="204"/>
+      <c r="G25" s="204"/>
+      <c r="H25" s="203"/>
+      <c r="I25" s="203"/>
+      <c r="J25" s="203"/>
+      <c r="K25" s="204"/>
+      <c r="L25" s="204"/>
+      <c r="M25" s="204"/>
+      <c r="N25" s="203"/>
+      <c r="O25" s="203"/>
+      <c r="P25" s="203"/>
+      <c r="Q25" s="204"/>
+      <c r="R25" s="204"/>
+      <c r="S25" s="204"/>
+      <c r="T25" s="204"/>
+      <c r="U25" s="212"/>
       <c r="AB25" s="44">
         <f>Consuntivo_2_PA!U22</f>
         <v>0</v>
@@ -13525,7 +13486,7 @@
         <f>Consuntivo_2_PA!AD22</f>
         <v>0</v>
       </c>
-      <c r="AL25" s="199"/>
+      <c r="AL25" s="193"/>
       <c r="AO25" s="5">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -13604,50 +13565,50 @@
       </c>
     </row>
     <row r="26" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A26" s="198" t="s">
+      <c r="A26" s="202" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="196">
+      <c r="B26" s="204">
         <f>SUM(AO5:AQ5,AO16:AQ17,AO33:AQ34,AO50:AQ51)</f>
         <v>13</v>
       </c>
-      <c r="C26" s="196"/>
-      <c r="D26" s="196"/>
-      <c r="E26" s="196">
+      <c r="C26" s="204"/>
+      <c r="D26" s="204"/>
+      <c r="E26" s="204">
         <f>SUM(AR5:AT5,AR16:AT17,AR33:AT34,AR50:AT51)</f>
         <v>10</v>
       </c>
-      <c r="F26" s="196"/>
-      <c r="G26" s="196"/>
-      <c r="H26" s="196">
+      <c r="F26" s="204"/>
+      <c r="G26" s="204"/>
+      <c r="H26" s="204">
         <f>SUM(AU5:AW5,AU16:AW17,AU33:AW34,AU50:AW51)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="196"/>
-      <c r="J26" s="196"/>
-      <c r="K26" s="197">
+      <c r="I26" s="204"/>
+      <c r="J26" s="204"/>
+      <c r="K26" s="203">
         <f>SUM(AX5:AZ5,AX16:AZ17,AX33:AZ34,AX50:AZ51)</f>
         <v>33</v>
       </c>
-      <c r="L26" s="197"/>
-      <c r="M26" s="197"/>
-      <c r="N26" s="196">
+      <c r="L26" s="203"/>
+      <c r="M26" s="203"/>
+      <c r="N26" s="204">
         <f>SUM(BA5:BC5,BA16:BC17,BA33:BC34,BA50:BC51)</f>
         <v>29</v>
       </c>
-      <c r="O26" s="196"/>
-      <c r="P26" s="196"/>
-      <c r="Q26" s="196">
+      <c r="O26" s="204"/>
+      <c r="P26" s="204"/>
+      <c r="Q26" s="204">
         <f>SUM(BD5:BF5,BD16:BF17,BD33:BF34,BD50:BF51)</f>
         <v>12</v>
       </c>
-      <c r="R26" s="196"/>
-      <c r="S26" s="196"/>
-      <c r="T26" s="196">
+      <c r="R26" s="204"/>
+      <c r="S26" s="204"/>
+      <c r="T26" s="204">
         <f t="shared" ref="T26" si="33">SUM(B26:S27)</f>
         <v>97</v>
       </c>
-      <c r="U26" s="193"/>
+      <c r="U26" s="212"/>
       <c r="AB26" s="53" t="str">
         <f>Consuntivo_2_PA!U23</f>
         <v>Maggiolo Giorgio</v>
@@ -13688,7 +13649,7 @@
         <f>Consuntivo_2_PA!AD23</f>
         <v>PA 3.3</v>
       </c>
-      <c r="AL26" s="199">
+      <c r="AL26" s="193">
         <f>Consuntivo_2_PA!AE23</f>
         <v>28</v>
       </c>
@@ -13770,27 +13731,27 @@
       </c>
     </row>
     <row r="27" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="198"/>
-      <c r="B27" s="196"/>
-      <c r="C27" s="196"/>
-      <c r="D27" s="196"/>
-      <c r="E27" s="196"/>
-      <c r="F27" s="196"/>
-      <c r="G27" s="196"/>
-      <c r="H27" s="196"/>
-      <c r="I27" s="196"/>
-      <c r="J27" s="196"/>
-      <c r="K27" s="197"/>
-      <c r="L27" s="197"/>
-      <c r="M27" s="197"/>
-      <c r="N27" s="196"/>
-      <c r="O27" s="196"/>
-      <c r="P27" s="196"/>
-      <c r="Q27" s="196"/>
-      <c r="R27" s="196"/>
-      <c r="S27" s="196"/>
-      <c r="T27" s="196"/>
-      <c r="U27" s="193"/>
+      <c r="A27" s="202"/>
+      <c r="B27" s="204"/>
+      <c r="C27" s="204"/>
+      <c r="D27" s="204"/>
+      <c r="E27" s="204"/>
+      <c r="F27" s="204"/>
+      <c r="G27" s="204"/>
+      <c r="H27" s="204"/>
+      <c r="I27" s="204"/>
+      <c r="J27" s="204"/>
+      <c r="K27" s="203"/>
+      <c r="L27" s="203"/>
+      <c r="M27" s="203"/>
+      <c r="N27" s="204"/>
+      <c r="O27" s="204"/>
+      <c r="P27" s="204"/>
+      <c r="Q27" s="204"/>
+      <c r="R27" s="204"/>
+      <c r="S27" s="204"/>
+      <c r="T27" s="204"/>
+      <c r="U27" s="212"/>
       <c r="AB27" s="75">
         <f>Consuntivo_2_PA!U24</f>
         <v>0</v>
@@ -13831,7 +13792,7 @@
         <f>Consuntivo_2_PA!AD24</f>
         <v>PA 5.1</v>
       </c>
-      <c r="AL27" s="213"/>
+      <c r="AL27" s="194"/>
       <c r="AO27" s="5">
         <f t="shared" si="29"/>
         <v>0</v>
@@ -13910,96 +13871,96 @@
       </c>
     </row>
     <row r="28" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="198" t="s">
+      <c r="A28" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="196">
+      <c r="B28" s="204">
         <f>SUM(AO6:AQ6,AO18:AQ19,AO35:AQ36,AO52:AQ53)</f>
         <v>10</v>
       </c>
-      <c r="C28" s="196"/>
-      <c r="D28" s="196"/>
-      <c r="E28" s="196">
+      <c r="C28" s="204"/>
+      <c r="D28" s="204"/>
+      <c r="E28" s="204">
         <f>SUM(AR6:AT6,AR18:AT19,AR35:AT36,AR52:AT53)</f>
         <v>4</v>
       </c>
-      <c r="F28" s="196"/>
-      <c r="G28" s="196"/>
-      <c r="H28" s="196">
+      <c r="F28" s="204"/>
+      <c r="G28" s="204"/>
+      <c r="H28" s="204">
         <f>SUM(AU6:AW6,AU18:AW19,AU35:AW36,AU52:AW53)</f>
         <v>2</v>
       </c>
-      <c r="I28" s="196"/>
-      <c r="J28" s="196"/>
-      <c r="K28" s="196">
+      <c r="I28" s="204"/>
+      <c r="J28" s="204"/>
+      <c r="K28" s="204">
         <f>SUM(AX6:AZ6,AX18:AZ19,AX35:AZ36,AX52:AZ53)</f>
         <v>27</v>
       </c>
-      <c r="L28" s="196"/>
-      <c r="M28" s="196"/>
-      <c r="N28" s="196">
+      <c r="L28" s="204"/>
+      <c r="M28" s="204"/>
+      <c r="N28" s="204">
         <f>SUM(BA6:BC6,BA18:BC19,BA35:BC36,BA52:BC53)</f>
         <v>33</v>
       </c>
-      <c r="O28" s="196"/>
-      <c r="P28" s="196"/>
-      <c r="Q28" s="197">
+      <c r="O28" s="204"/>
+      <c r="P28" s="204"/>
+      <c r="Q28" s="203">
         <f>SUM(BD6:BF6,BD18:BF19,BD35:BF36,BD52:BF53)</f>
         <v>20</v>
       </c>
-      <c r="R28" s="197"/>
-      <c r="S28" s="197"/>
-      <c r="T28" s="196">
+      <c r="R28" s="203"/>
+      <c r="S28" s="203"/>
+      <c r="T28" s="204">
         <f t="shared" ref="T28" si="34">SUM(B28:S29)</f>
         <v>96</v>
       </c>
-      <c r="U28" s="193"/>
+      <c r="U28" s="212"/>
       <c r="BG28" s="144">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A29" s="198"/>
-      <c r="B29" s="196"/>
-      <c r="C29" s="196"/>
-      <c r="D29" s="196"/>
-      <c r="E29" s="196"/>
-      <c r="F29" s="196"/>
-      <c r="G29" s="196"/>
-      <c r="H29" s="196"/>
-      <c r="I29" s="196"/>
-      <c r="J29" s="196"/>
-      <c r="K29" s="196"/>
-      <c r="L29" s="196"/>
-      <c r="M29" s="196"/>
-      <c r="N29" s="196"/>
-      <c r="O29" s="196"/>
-      <c r="P29" s="196"/>
-      <c r="Q29" s="197"/>
-      <c r="R29" s="197"/>
-      <c r="S29" s="197"/>
-      <c r="T29" s="196"/>
-      <c r="U29" s="193"/>
+      <c r="A29" s="202"/>
+      <c r="B29" s="204"/>
+      <c r="C29" s="204"/>
+      <c r="D29" s="204"/>
+      <c r="E29" s="204"/>
+      <c r="F29" s="204"/>
+      <c r="G29" s="204"/>
+      <c r="H29" s="204"/>
+      <c r="I29" s="204"/>
+      <c r="J29" s="204"/>
+      <c r="K29" s="204"/>
+      <c r="L29" s="204"/>
+      <c r="M29" s="204"/>
+      <c r="N29" s="204"/>
+      <c r="O29" s="204"/>
+      <c r="P29" s="204"/>
+      <c r="Q29" s="203"/>
+      <c r="R29" s="203"/>
+      <c r="S29" s="203"/>
+      <c r="T29" s="204"/>
+      <c r="U29" s="212"/>
       <c r="AA29" s="5" t="s">
         <v>124</v>
       </c>
       <c r="AB29" s="140" t="s">
         <v>127</v>
       </c>
-      <c r="AC29" s="207" t="str">
+      <c r="AC29" s="195" t="str">
         <f>'3_PDC'!U6</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD29" s="208"/>
-      <c r="AE29" s="209"/>
-      <c r="AF29" s="207" t="str">
+      <c r="AD29" s="196"/>
+      <c r="AE29" s="197"/>
+      <c r="AF29" s="195" t="str">
         <f>'3_PDC'!X6</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG29" s="208"/>
-      <c r="AH29" s="210"/>
-      <c r="AI29" s="203" t="str">
+      <c r="AG29" s="196"/>
+      <c r="AH29" s="198"/>
+      <c r="AI29" s="199" t="str">
         <f>'3_PDC'!AA6</f>
         <v>Totale</v>
       </c>
@@ -14009,50 +13970,50 @@
       </c>
     </row>
     <row r="30" spans="1:60" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="198" t="s">
+      <c r="A30" s="202" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="196">
+      <c r="B30" s="204">
         <f>SUM(AO7:AQ7,AO20:AQ21,AO37:AQ38,AO54:AQ55)</f>
         <v>15</v>
       </c>
-      <c r="C30" s="196"/>
-      <c r="D30" s="196"/>
-      <c r="E30" s="196">
+      <c r="C30" s="204"/>
+      <c r="D30" s="204"/>
+      <c r="E30" s="204">
         <f>SUM(AR7:AT7,AR20:AT21,AR37:AT38,AR54:AT55)</f>
         <v>4</v>
       </c>
-      <c r="F30" s="196"/>
-      <c r="G30" s="196"/>
-      <c r="H30" s="196">
+      <c r="F30" s="204"/>
+      <c r="G30" s="204"/>
+      <c r="H30" s="204">
         <f>SUM(AU7:AW7,AU20:AW21,AU37:AW38,AU54:AW55)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="196"/>
-      <c r="J30" s="196"/>
-      <c r="K30" s="197">
+      <c r="I30" s="204"/>
+      <c r="J30" s="204"/>
+      <c r="K30" s="203">
         <f>SUM(AX7:AZ7,AX20:AZ21,AX37:AZ38,AX54:AZ55)</f>
         <v>31</v>
       </c>
-      <c r="L30" s="197"/>
-      <c r="M30" s="197"/>
-      <c r="N30" s="197">
+      <c r="L30" s="203"/>
+      <c r="M30" s="203"/>
+      <c r="N30" s="203">
         <f>SUM(BA7:BC7,BA20:BC21,BA37:BC38,BA54:BC55)</f>
         <v>35</v>
       </c>
-      <c r="O30" s="197"/>
-      <c r="P30" s="197"/>
-      <c r="Q30" s="196">
+      <c r="O30" s="203"/>
+      <c r="P30" s="203"/>
+      <c r="Q30" s="204">
         <f>SUM(BD7:BF7,BD20:BF21,BD37:BF38,BD54:BF55)</f>
         <v>18</v>
       </c>
-      <c r="R30" s="196"/>
-      <c r="S30" s="196"/>
-      <c r="T30" s="196">
+      <c r="R30" s="204"/>
+      <c r="S30" s="204"/>
+      <c r="T30" s="204">
         <f t="shared" ref="T30" si="35">SUM(B30:S31)</f>
         <v>103</v>
       </c>
-      <c r="U30" s="193"/>
+      <c r="U30" s="212"/>
       <c r="AB30" s="141"/>
       <c r="AC30" s="40" t="str">
         <f>'3_PDC'!U7</f>
@@ -14078,7 +14039,7 @@
         <f>'3_PDC'!Z7</f>
         <v>Fase</v>
       </c>
-      <c r="AI30" s="204"/>
+      <c r="AI30" s="200"/>
       <c r="AK30" s="5">
         <f>SUM(AI31:AI44)</f>
         <v>373</v>
@@ -14089,27 +14050,27 @@
       </c>
     </row>
     <row r="31" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A31" s="198"/>
-      <c r="B31" s="196"/>
-      <c r="C31" s="196"/>
-      <c r="D31" s="196"/>
-      <c r="E31" s="196"/>
-      <c r="F31" s="196"/>
-      <c r="G31" s="196"/>
-      <c r="H31" s="196"/>
-      <c r="I31" s="196"/>
-      <c r="J31" s="196"/>
-      <c r="K31" s="197"/>
-      <c r="L31" s="197"/>
-      <c r="M31" s="197"/>
-      <c r="N31" s="197"/>
-      <c r="O31" s="197"/>
-      <c r="P31" s="197"/>
-      <c r="Q31" s="196"/>
-      <c r="R31" s="196"/>
-      <c r="S31" s="196"/>
-      <c r="T31" s="196"/>
-      <c r="U31" s="193"/>
+      <c r="A31" s="202"/>
+      <c r="B31" s="204"/>
+      <c r="C31" s="204"/>
+      <c r="D31" s="204"/>
+      <c r="E31" s="204"/>
+      <c r="F31" s="204"/>
+      <c r="G31" s="204"/>
+      <c r="H31" s="204"/>
+      <c r="I31" s="204"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="203"/>
+      <c r="L31" s="203"/>
+      <c r="M31" s="203"/>
+      <c r="N31" s="203"/>
+      <c r="O31" s="203"/>
+      <c r="P31" s="203"/>
+      <c r="Q31" s="204"/>
+      <c r="R31" s="204"/>
+      <c r="S31" s="204"/>
+      <c r="T31" s="204"/>
+      <c r="U31" s="212"/>
       <c r="AB31" s="44" t="str">
         <f>'3_PDC'!T8</f>
         <v>Begolo Marco</v>
@@ -14138,7 +14099,7 @@
         <f>'3_PDC'!Z8</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI31" s="211">
+      <c r="AI31" s="201">
         <f>'3_PDC'!AA8</f>
         <v>52</v>
       </c>
@@ -14224,50 +14185,50 @@
       </c>
     </row>
     <row r="32" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A32" s="198" t="s">
+      <c r="A32" s="202" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="196">
+      <c r="B32" s="204">
         <f>SUM(AO8:AQ8,AO22:AQ23,AO39:AQ40,AO56:AQ57)</f>
         <v>9</v>
       </c>
-      <c r="C32" s="196"/>
-      <c r="D32" s="196"/>
-      <c r="E32" s="196">
+      <c r="C32" s="204"/>
+      <c r="D32" s="204"/>
+      <c r="E32" s="204">
         <f>SUM(AR8:AT8,AR22:AT23,AR39:AT40,AR56:AT57)</f>
         <v>11</v>
       </c>
-      <c r="F32" s="196"/>
-      <c r="G32" s="196"/>
-      <c r="H32" s="196">
+      <c r="F32" s="204"/>
+      <c r="G32" s="204"/>
+      <c r="H32" s="204">
         <f>SUM(AU8:AW8,AU22:AW23,AU39:AW40,AU56:AW57)</f>
         <v>2</v>
       </c>
-      <c r="I32" s="196"/>
-      <c r="J32" s="196"/>
-      <c r="K32" s="196">
+      <c r="I32" s="204"/>
+      <c r="J32" s="204"/>
+      <c r="K32" s="204">
         <f>SUM(AX8:AZ8,AX22:AZ23,AX39:AZ40,AX56:AZ57)</f>
         <v>20</v>
       </c>
-      <c r="L32" s="196"/>
-      <c r="M32" s="196"/>
-      <c r="N32" s="197">
+      <c r="L32" s="204"/>
+      <c r="M32" s="204"/>
+      <c r="N32" s="203">
         <f>SUM(BA8:BC8,BA22:BC23,BA39:BC40,BA56:BC57)</f>
         <v>37</v>
       </c>
-      <c r="O32" s="197"/>
-      <c r="P32" s="197"/>
-      <c r="Q32" s="196">
+      <c r="O32" s="203"/>
+      <c r="P32" s="203"/>
+      <c r="Q32" s="204">
         <f>SUM(BD8:BF8,BD22:BF23,BD39:BF40,BD56:BF57)</f>
         <v>23</v>
       </c>
-      <c r="R32" s="196"/>
-      <c r="S32" s="196"/>
-      <c r="T32" s="196">
+      <c r="R32" s="204"/>
+      <c r="S32" s="204"/>
+      <c r="T32" s="204">
         <f t="shared" ref="T32" si="51">SUM(B32:S33)</f>
         <v>102</v>
       </c>
-      <c r="U32" s="193"/>
+      <c r="U32" s="212"/>
       <c r="AB32" s="49">
         <f>'3_PDC'!T9</f>
         <v>0</v>
@@ -14296,7 +14257,7 @@
         <f>'3_PDC'!Z9</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI32" s="199"/>
+      <c r="AI32" s="193"/>
       <c r="AO32" s="5">
         <f>IF($AC32=AO$2,$AD32,0)</f>
         <v>0</v>
@@ -14375,27 +14336,27 @@
       </c>
     </row>
     <row r="33" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A33" s="198"/>
-      <c r="B33" s="196"/>
-      <c r="C33" s="196"/>
-      <c r="D33" s="196"/>
-      <c r="E33" s="196"/>
-      <c r="F33" s="196"/>
-      <c r="G33" s="196"/>
-      <c r="H33" s="196"/>
-      <c r="I33" s="196"/>
-      <c r="J33" s="196"/>
-      <c r="K33" s="196"/>
-      <c r="L33" s="196"/>
-      <c r="M33" s="196"/>
-      <c r="N33" s="197"/>
-      <c r="O33" s="197"/>
-      <c r="P33" s="197"/>
-      <c r="Q33" s="196"/>
-      <c r="R33" s="196"/>
-      <c r="S33" s="196"/>
-      <c r="T33" s="196"/>
-      <c r="U33" s="193"/>
+      <c r="A33" s="202"/>
+      <c r="B33" s="204"/>
+      <c r="C33" s="204"/>
+      <c r="D33" s="204"/>
+      <c r="E33" s="204"/>
+      <c r="F33" s="204"/>
+      <c r="G33" s="204"/>
+      <c r="H33" s="204"/>
+      <c r="I33" s="204"/>
+      <c r="J33" s="204"/>
+      <c r="K33" s="204"/>
+      <c r="L33" s="204"/>
+      <c r="M33" s="204"/>
+      <c r="N33" s="203"/>
+      <c r="O33" s="203"/>
+      <c r="P33" s="203"/>
+      <c r="Q33" s="204"/>
+      <c r="R33" s="204"/>
+      <c r="S33" s="204"/>
+      <c r="T33" s="204"/>
+      <c r="U33" s="212"/>
       <c r="AB33" s="44" t="str">
         <f>'3_PDC'!T10</f>
         <v>Facchin Gabriele</v>
@@ -14424,7 +14385,7 @@
         <f>'3_PDC'!Z10</f>
         <v>PDC 3.1</v>
       </c>
-      <c r="AI33" s="199">
+      <c r="AI33" s="193">
         <f>'3_PDC'!AA10</f>
         <v>52</v>
       </c>
@@ -14506,50 +14467,50 @@
       </c>
     </row>
     <row r="34" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A34" s="198" t="s">
+      <c r="A34" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="196">
+      <c r="B34" s="204">
         <f>SUM(AO9:AQ9,AO24:AQ25,AO41:AQ42,AO58:AQ59)</f>
         <v>6</v>
       </c>
-      <c r="C34" s="196"/>
-      <c r="D34" s="196"/>
-      <c r="E34" s="196">
+      <c r="C34" s="204"/>
+      <c r="D34" s="204"/>
+      <c r="E34" s="204">
         <f>SUM(AR9:AT9,AR24:AT25,AR41:AT42,AR58:AT59)</f>
         <v>2</v>
       </c>
-      <c r="F34" s="196"/>
-      <c r="G34" s="196"/>
-      <c r="H34" s="196">
+      <c r="F34" s="204"/>
+      <c r="G34" s="204"/>
+      <c r="H34" s="204">
         <f>SUM(AU9:AW9,AU24:AW25,AU41:AW42,AU58:AW59)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="196"/>
-      <c r="J34" s="196"/>
-      <c r="K34" s="197">
+      <c r="I34" s="204"/>
+      <c r="J34" s="204"/>
+      <c r="K34" s="203">
         <f>SUM(AX9:AZ9,AX24:AZ25,AX41:AZ42,AX58:AZ59)</f>
         <v>27</v>
       </c>
-      <c r="L34" s="197"/>
-      <c r="M34" s="197"/>
-      <c r="N34" s="197">
+      <c r="L34" s="203"/>
+      <c r="M34" s="203"/>
+      <c r="N34" s="203">
         <f>SUM(BA9:BC9,BA24:BC25,BA41:BC42,BA58:BC59)</f>
         <v>40</v>
       </c>
-      <c r="O34" s="197"/>
-      <c r="P34" s="197"/>
-      <c r="Q34" s="197">
+      <c r="O34" s="203"/>
+      <c r="P34" s="203"/>
+      <c r="Q34" s="203">
         <f>SUM(BD9:BF9,BD24:BF25,BD41:BF42,BD58:BF59)</f>
         <v>25</v>
       </c>
-      <c r="R34" s="197"/>
-      <c r="S34" s="197"/>
-      <c r="T34" s="196">
+      <c r="R34" s="203"/>
+      <c r="S34" s="203"/>
+      <c r="T34" s="204">
         <f t="shared" ref="T34" si="55">SUM(B34:S35)</f>
         <v>100</v>
       </c>
-      <c r="U34" s="193"/>
+      <c r="U34" s="212"/>
       <c r="AB34" s="44">
         <f>'3_PDC'!T11</f>
         <v>0</v>
@@ -14578,7 +14539,7 @@
         <f>'3_PDC'!Z11</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI34" s="199"/>
+      <c r="AI34" s="193"/>
       <c r="AO34" s="5">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -14657,27 +14618,27 @@
       </c>
     </row>
     <row r="35" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A35" s="198"/>
-      <c r="B35" s="196"/>
-      <c r="C35" s="196"/>
-      <c r="D35" s="196"/>
-      <c r="E35" s="196"/>
-      <c r="F35" s="196"/>
-      <c r="G35" s="196"/>
-      <c r="H35" s="196"/>
-      <c r="I35" s="196"/>
-      <c r="J35" s="196"/>
-      <c r="K35" s="197"/>
-      <c r="L35" s="197"/>
-      <c r="M35" s="197"/>
-      <c r="N35" s="197"/>
-      <c r="O35" s="197"/>
-      <c r="P35" s="197"/>
-      <c r="Q35" s="197"/>
-      <c r="R35" s="197"/>
-      <c r="S35" s="197"/>
-      <c r="T35" s="196"/>
-      <c r="U35" s="193"/>
+      <c r="A35" s="202"/>
+      <c r="B35" s="204"/>
+      <c r="C35" s="204"/>
+      <c r="D35" s="204"/>
+      <c r="E35" s="204"/>
+      <c r="F35" s="204"/>
+      <c r="G35" s="204"/>
+      <c r="H35" s="204"/>
+      <c r="I35" s="204"/>
+      <c r="J35" s="204"/>
+      <c r="K35" s="203"/>
+      <c r="L35" s="203"/>
+      <c r="M35" s="203"/>
+      <c r="N35" s="203"/>
+      <c r="O35" s="203"/>
+      <c r="P35" s="203"/>
+      <c r="Q35" s="203"/>
+      <c r="R35" s="203"/>
+      <c r="S35" s="203"/>
+      <c r="T35" s="204"/>
+      <c r="U35" s="212"/>
       <c r="AB35" s="53" t="str">
         <f>'3_PDC'!T12</f>
         <v>Cornaglia Alessando</v>
@@ -14706,7 +14667,7 @@
         <f>'3_PDC'!Z12</f>
         <v>PDC 4.4 e 5</v>
       </c>
-      <c r="AI35" s="199">
+      <c r="AI35" s="193">
         <f>'3_PDC'!AA12</f>
         <v>52</v>
       </c>
@@ -14795,50 +14756,50 @@
       </c>
     </row>
     <row r="36" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A36" s="198" t="s">
+      <c r="A36" s="202" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="196">
+      <c r="B36" s="204">
         <f>SUM(AO10:AQ10,AO26:AQ27,AO43:AQ44,AO60:AQ61)</f>
         <v>2</v>
       </c>
-      <c r="C36" s="196"/>
-      <c r="D36" s="196"/>
-      <c r="E36" s="196">
+      <c r="C36" s="204"/>
+      <c r="D36" s="204"/>
+      <c r="E36" s="204">
         <f>SUM(AR10:AT10,AR26:AT27,AR43:AT44,AR60:AT61)</f>
         <v>8</v>
       </c>
-      <c r="F36" s="196"/>
-      <c r="G36" s="196"/>
-      <c r="H36" s="196">
+      <c r="F36" s="204"/>
+      <c r="G36" s="204"/>
+      <c r="H36" s="204">
         <f>SUM(AU10:AW10,AU26:AW27,AU43:AW44,AU60:AW61)</f>
         <v>7</v>
       </c>
-      <c r="I36" s="196"/>
-      <c r="J36" s="196"/>
-      <c r="K36" s="197">
+      <c r="I36" s="204"/>
+      <c r="J36" s="204"/>
+      <c r="K36" s="203">
         <f>SUM(AX10:AZ10,AX26:AZ27,AX43:AZ44,AX60:AZ61)</f>
         <v>51</v>
       </c>
-      <c r="L36" s="197"/>
-      <c r="M36" s="197"/>
-      <c r="N36" s="196">
+      <c r="L36" s="203"/>
+      <c r="M36" s="203"/>
+      <c r="N36" s="204">
         <f>SUM(BA10:BC10,BA26:BC27,BA43:BC44,BA60:BC61)</f>
         <v>10</v>
       </c>
-      <c r="O36" s="196"/>
-      <c r="P36" s="196"/>
-      <c r="Q36" s="196">
+      <c r="O36" s="204"/>
+      <c r="P36" s="204"/>
+      <c r="Q36" s="204">
         <f>SUM(BD10:BF10,BD26:BF27,BD43:BF44,BD60:BF61)</f>
         <v>18</v>
       </c>
-      <c r="R36" s="196"/>
-      <c r="S36" s="196"/>
-      <c r="T36" s="196">
+      <c r="R36" s="204"/>
+      <c r="S36" s="204"/>
+      <c r="T36" s="204">
         <f t="shared" ref="T36" si="56">SUM(B36:S37)</f>
         <v>96</v>
       </c>
-      <c r="U36" s="193"/>
+      <c r="U36" s="212"/>
       <c r="AB36" s="49">
         <f>'3_PDC'!T13</f>
         <v>0</v>
@@ -14867,7 +14828,7 @@
         <f>'3_PDC'!Z13</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI36" s="199"/>
+      <c r="AI36" s="193"/>
       <c r="AK36" s="5">
         <f>SUM(BD31:BF44)</f>
         <v>100</v>
@@ -14950,27 +14911,27 @@
       </c>
     </row>
     <row r="37" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A37" s="198"/>
-      <c r="B37" s="196"/>
-      <c r="C37" s="196"/>
-      <c r="D37" s="196"/>
-      <c r="E37" s="196"/>
-      <c r="F37" s="196"/>
-      <c r="G37" s="196"/>
-      <c r="H37" s="196"/>
-      <c r="I37" s="196"/>
-      <c r="J37" s="196"/>
-      <c r="K37" s="197"/>
-      <c r="L37" s="197"/>
-      <c r="M37" s="197"/>
-      <c r="N37" s="196"/>
-      <c r="O37" s="196"/>
-      <c r="P37" s="196"/>
-      <c r="Q37" s="196"/>
-      <c r="R37" s="196"/>
-      <c r="S37" s="196"/>
-      <c r="T37" s="196"/>
-      <c r="U37" s="193"/>
+      <c r="A37" s="202"/>
+      <c r="B37" s="204"/>
+      <c r="C37" s="204"/>
+      <c r="D37" s="204"/>
+      <c r="E37" s="204"/>
+      <c r="F37" s="204"/>
+      <c r="G37" s="204"/>
+      <c r="H37" s="204"/>
+      <c r="I37" s="204"/>
+      <c r="J37" s="204"/>
+      <c r="K37" s="203"/>
+      <c r="L37" s="203"/>
+      <c r="M37" s="203"/>
+      <c r="N37" s="204"/>
+      <c r="O37" s="204"/>
+      <c r="P37" s="204"/>
+      <c r="Q37" s="204"/>
+      <c r="R37" s="204"/>
+      <c r="S37" s="204"/>
+      <c r="T37" s="204"/>
+      <c r="U37" s="212"/>
       <c r="AB37" s="44" t="str">
         <f>'3_PDC'!T14</f>
         <v>Dalla Pietà Massimo</v>
@@ -14999,7 +14960,7 @@
         <f>'3_PDC'!Z14</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI37" s="199">
+      <c r="AI37" s="193">
         <f>'3_PDC'!AA14</f>
         <v>57</v>
       </c>
@@ -15081,50 +15042,50 @@
       </c>
     </row>
     <row r="38" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A38" s="195" t="s">
+      <c r="A38" s="211" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="196">
+      <c r="B38" s="204">
         <f>SUM(B24:D37)</f>
         <v>59</v>
       </c>
-      <c r="C38" s="196"/>
-      <c r="D38" s="196"/>
-      <c r="E38" s="196">
+      <c r="C38" s="204"/>
+      <c r="D38" s="204"/>
+      <c r="E38" s="204">
         <f t="shared" ref="E38" si="57">SUM(E24:G37)</f>
         <v>49</v>
       </c>
-      <c r="F38" s="196"/>
-      <c r="G38" s="196"/>
-      <c r="H38" s="196">
+      <c r="F38" s="204"/>
+      <c r="G38" s="204"/>
+      <c r="H38" s="204">
         <f>SUM(H24:J37)</f>
         <v>20</v>
       </c>
-      <c r="I38" s="196"/>
-      <c r="J38" s="196"/>
-      <c r="K38" s="196">
+      <c r="I38" s="204"/>
+      <c r="J38" s="204"/>
+      <c r="K38" s="204">
         <f t="shared" ref="K38" si="58">SUM(K24:M37)</f>
         <v>199</v>
       </c>
-      <c r="L38" s="196"/>
-      <c r="M38" s="196"/>
-      <c r="N38" s="196">
+      <c r="L38" s="204"/>
+      <c r="M38" s="204"/>
+      <c r="N38" s="204">
         <f t="shared" ref="N38" si="59">SUM(N24:P37)</f>
         <v>243</v>
       </c>
-      <c r="O38" s="196"/>
-      <c r="P38" s="196"/>
-      <c r="Q38" s="196">
+      <c r="O38" s="204"/>
+      <c r="P38" s="204"/>
+      <c r="Q38" s="204">
         <f>SUM(Q24:S37)</f>
         <v>120</v>
       </c>
-      <c r="R38" s="196"/>
-      <c r="S38" s="196"/>
-      <c r="T38" s="196">
+      <c r="R38" s="204"/>
+      <c r="S38" s="204"/>
+      <c r="T38" s="204">
         <f>SUM(B38:S39)</f>
         <v>690</v>
       </c>
-      <c r="U38" s="193"/>
+      <c r="U38" s="212"/>
       <c r="AB38" s="44">
         <f>'3_PDC'!T15</f>
         <v>0</v>
@@ -15153,7 +15114,7 @@
         <f>'3_PDC'!Z15</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI38" s="199"/>
+      <c r="AI38" s="193"/>
       <c r="AO38" s="5">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -15232,27 +15193,27 @@
       </c>
     </row>
     <row r="39" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A39" s="195"/>
-      <c r="B39" s="196"/>
-      <c r="C39" s="196"/>
-      <c r="D39" s="196"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="196"/>
-      <c r="H39" s="196"/>
-      <c r="I39" s="196"/>
-      <c r="J39" s="196"/>
-      <c r="K39" s="196"/>
-      <c r="L39" s="196"/>
-      <c r="M39" s="196"/>
-      <c r="N39" s="196"/>
-      <c r="O39" s="196"/>
-      <c r="P39" s="196"/>
-      <c r="Q39" s="196"/>
-      <c r="R39" s="196"/>
-      <c r="S39" s="196"/>
-      <c r="T39" s="196"/>
-      <c r="U39" s="193"/>
+      <c r="A39" s="211"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="204"/>
+      <c r="D39" s="204"/>
+      <c r="E39" s="204"/>
+      <c r="F39" s="204"/>
+      <c r="G39" s="204"/>
+      <c r="H39" s="204"/>
+      <c r="I39" s="204"/>
+      <c r="J39" s="204"/>
+      <c r="K39" s="204"/>
+      <c r="L39" s="204"/>
+      <c r="M39" s="204"/>
+      <c r="N39" s="204"/>
+      <c r="O39" s="204"/>
+      <c r="P39" s="204"/>
+      <c r="Q39" s="204"/>
+      <c r="R39" s="204"/>
+      <c r="S39" s="204"/>
+      <c r="T39" s="204"/>
+      <c r="U39" s="212"/>
       <c r="AB39" s="53" t="str">
         <f>'3_PDC'!T16</f>
         <v>Braghetto Lorenzo</v>
@@ -15281,7 +15242,7 @@
         <f>'3_PDC'!Z16</f>
         <v>PDC 4.4</v>
       </c>
-      <c r="AI39" s="199">
+      <c r="AI39" s="193">
         <f>'3_PDC'!AA16</f>
         <v>54</v>
       </c>
@@ -15392,7 +15353,7 @@
         <f>'3_PDC'!Z17</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI40" s="199"/>
+      <c r="AI40" s="193"/>
       <c r="AO40" s="5">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -15500,7 +15461,7 @@
         <f>'3_PDC'!Z18</f>
         <v>PDC 6</v>
       </c>
-      <c r="AI41" s="199">
+      <c r="AI41" s="193">
         <f>'3_PDC'!AA18</f>
         <v>54</v>
       </c>
@@ -15611,7 +15572,7 @@
         <f>'3_PDC'!Z19</f>
         <v>PDC 3.2, 5 e 7</v>
       </c>
-      <c r="AI42" s="199"/>
+      <c r="AI42" s="193"/>
       <c r="AO42" s="5">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -15719,7 +15680,7 @@
         <f>'3_PDC'!Z20</f>
         <v>PDC 4.3</v>
       </c>
-      <c r="AI43" s="199">
+      <c r="AI43" s="193">
         <f>'3_PDC'!AA20</f>
         <v>52</v>
       </c>
@@ -15830,7 +15791,7 @@
         <f>'3_PDC'!Z21</f>
         <v>PDC 7</v>
       </c>
-      <c r="AI44" s="213"/>
+      <c r="AI44" s="194"/>
       <c r="AO44" s="5">
         <f t="shared" si="52"/>
         <v>0</v>
@@ -15923,19 +15884,19 @@
       <c r="AB46" s="140" t="s">
         <v>128</v>
       </c>
-      <c r="AC46" s="207" t="str">
+      <c r="AC46" s="195" t="str">
         <f>'4_VV'!U3</f>
         <v>I Periodo</v>
       </c>
-      <c r="AD46" s="208"/>
-      <c r="AE46" s="209"/>
-      <c r="AF46" s="207" t="str">
+      <c r="AD46" s="196"/>
+      <c r="AE46" s="197"/>
+      <c r="AF46" s="195" t="str">
         <f>'4_VV'!X3</f>
         <v>II Periodo</v>
       </c>
-      <c r="AG46" s="208"/>
-      <c r="AH46" s="210"/>
-      <c r="AI46" s="203" t="str">
+      <c r="AG46" s="196"/>
+      <c r="AH46" s="198"/>
+      <c r="AI46" s="199" t="str">
         <f>'4_VV'!AA3</f>
         <v>Totale</v>
       </c>
@@ -15975,7 +15936,7 @@
         <f>'4_VV'!Z4</f>
         <v>Fase</v>
       </c>
-      <c r="AI47" s="204"/>
+      <c r="AI47" s="200"/>
       <c r="BG47" s="144">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -16011,7 +15972,7 @@
         <f>'4_VV'!Z5</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI48" s="211">
+      <c r="AI48" s="201">
         <f>'4_VV'!AA5</f>
         <v>18</v>
       </c>
@@ -16125,7 +16086,7 @@
         <f>'4_VV'!Z6</f>
         <v>0</v>
       </c>
-      <c r="AI49" s="199"/>
+      <c r="AI49" s="193"/>
       <c r="AO49" s="5">
         <f>IF($AC49=AO$2,$AD49,0)</f>
         <v>0</v>
@@ -16232,7 +16193,7 @@
         <f>'4_VV'!Z7</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI50" s="199">
+      <c r="AI50" s="193">
         <f>'4_VV'!AA7</f>
         <v>18</v>
       </c>
@@ -16361,7 +16322,7 @@
         <f>'4_VV'!Z8</f>
         <v>VV 3.2</v>
       </c>
-      <c r="AI51" s="199"/>
+      <c r="AI51" s="193"/>
       <c r="AO51" s="5">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16482,7 +16443,7 @@
         <f>'4_VV'!Z9</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI52" s="199">
+      <c r="AI52" s="193">
         <f>'4_VV'!AA9</f>
         <v>18</v>
       </c>
@@ -16606,7 +16567,7 @@
         <f>'4_VV'!Z10</f>
         <v>0</v>
       </c>
-      <c r="AI53" s="199"/>
+      <c r="AI53" s="193"/>
       <c r="AO53" s="5">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16727,7 +16688,7 @@
         <f>'4_VV'!Z11</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI54" s="199">
+      <c r="AI54" s="193">
         <f>'4_VV'!AA11</f>
         <v>18</v>
       </c>
@@ -16851,7 +16812,7 @@
         <f>'4_VV'!Z12</f>
         <v>0</v>
       </c>
-      <c r="AI55" s="199"/>
+      <c r="AI55" s="193"/>
       <c r="AO55" s="5">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -16972,7 +16933,7 @@
         <f>'4_VV'!Z13</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI56" s="199">
+      <c r="AI56" s="193">
         <f>'4_VV'!AA13</f>
         <v>18</v>
       </c>
@@ -17096,7 +17057,7 @@
         <f>'4_VV'!Z14</f>
         <v>0</v>
       </c>
-      <c r="AI57" s="199"/>
+      <c r="AI57" s="193"/>
       <c r="AO57" s="5">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -17214,7 +17175,7 @@
         <f>'4_VV'!Z15</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI58" s="199">
+      <c r="AI58" s="193">
         <f>'4_VV'!AA15</f>
         <v>18</v>
       </c>
@@ -17324,7 +17285,7 @@
         <f>'4_VV'!Z16</f>
         <v>0</v>
       </c>
-      <c r="AI59" s="199"/>
+      <c r="AI59" s="193"/>
       <c r="AO59" s="5">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -17431,7 +17392,7 @@
         <f>'4_VV'!Z17</f>
         <v>VV 3.1</v>
       </c>
-      <c r="AI60" s="199">
+      <c r="AI60" s="193">
         <f>'4_VV'!AA17</f>
         <v>16</v>
       </c>
@@ -17541,7 +17502,7 @@
         <f>'4_VV'!Z18</f>
         <v>0</v>
       </c>
-      <c r="AI61" s="213"/>
+      <c r="AI61" s="194"/>
       <c r="AO61" s="5">
         <f t="shared" si="75"/>
         <v>0</v>
@@ -17621,18 +17582,82 @@
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AC12:AE12"/>
-    <mergeCell ref="AF12:AH12"/>
-    <mergeCell ref="AI12:AK12"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:S23"/>
+    <mergeCell ref="AI56:AI57"/>
+    <mergeCell ref="AI58:AI59"/>
+    <mergeCell ref="AI60:AI61"/>
+    <mergeCell ref="AC46:AE46"/>
+    <mergeCell ref="AF46:AH46"/>
+    <mergeCell ref="AI46:AI47"/>
+    <mergeCell ref="AI48:AI49"/>
+    <mergeCell ref="AI50:AI51"/>
+    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="AI39:AI40"/>
+    <mergeCell ref="AI41:AI42"/>
+    <mergeCell ref="AI43:AI44"/>
+    <mergeCell ref="Q36:S37"/>
+    <mergeCell ref="T36:T37"/>
+    <mergeCell ref="U36:U37"/>
+    <mergeCell ref="AI37:AI38"/>
+    <mergeCell ref="AI35:AI36"/>
+    <mergeCell ref="AI54:AI55"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:D39"/>
+    <mergeCell ref="E38:G39"/>
+    <mergeCell ref="H38:J39"/>
+    <mergeCell ref="K38:M39"/>
+    <mergeCell ref="N38:P39"/>
+    <mergeCell ref="Q34:S35"/>
+    <mergeCell ref="T34:T35"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:D37"/>
+    <mergeCell ref="E36:G37"/>
+    <mergeCell ref="H36:J37"/>
+    <mergeCell ref="K36:M37"/>
+    <mergeCell ref="N36:P37"/>
+    <mergeCell ref="Q38:S39"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:D35"/>
+    <mergeCell ref="E34:G35"/>
+    <mergeCell ref="H34:J35"/>
+    <mergeCell ref="K34:M35"/>
+    <mergeCell ref="N34:P35"/>
+    <mergeCell ref="B24:D25"/>
+    <mergeCell ref="E24:G25"/>
+    <mergeCell ref="H24:J25"/>
+    <mergeCell ref="K24:M25"/>
+    <mergeCell ref="N24:P25"/>
+    <mergeCell ref="AC29:AE29"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D33"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="H32:J33"/>
+    <mergeCell ref="K32:M33"/>
+    <mergeCell ref="N32:P33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:D31"/>
+    <mergeCell ref="E30:G31"/>
+    <mergeCell ref="H30:J31"/>
+    <mergeCell ref="K30:M31"/>
+    <mergeCell ref="N30:P31"/>
+    <mergeCell ref="AF29:AH29"/>
+    <mergeCell ref="AI29:AI30"/>
+    <mergeCell ref="Q30:S31"/>
+    <mergeCell ref="T30:T31"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="AI31:AI32"/>
+    <mergeCell ref="Q26:S27"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="U26:U27"/>
+    <mergeCell ref="Q32:S33"/>
+    <mergeCell ref="T32:T33"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="AI33:AI34"/>
+    <mergeCell ref="Q28:S29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="U28:U29"/>
     <mergeCell ref="AL12:AL13"/>
     <mergeCell ref="AL14:AL15"/>
     <mergeCell ref="AL16:AL17"/>
@@ -17657,82 +17682,18 @@
     <mergeCell ref="K26:M27"/>
     <mergeCell ref="N26:P27"/>
     <mergeCell ref="A24:A25"/>
-    <mergeCell ref="AF29:AH29"/>
-    <mergeCell ref="AI29:AI30"/>
-    <mergeCell ref="Q30:S31"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="AI31:AI32"/>
-    <mergeCell ref="Q26:S27"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="U26:U27"/>
-    <mergeCell ref="Q32:S33"/>
-    <mergeCell ref="T32:T33"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="AI33:AI34"/>
-    <mergeCell ref="Q28:S29"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="B24:D25"/>
-    <mergeCell ref="E24:G25"/>
-    <mergeCell ref="H24:J25"/>
-    <mergeCell ref="K24:M25"/>
-    <mergeCell ref="N24:P25"/>
-    <mergeCell ref="AC29:AE29"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D33"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="H32:J33"/>
-    <mergeCell ref="K32:M33"/>
-    <mergeCell ref="N32:P33"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:D31"/>
-    <mergeCell ref="E30:G31"/>
-    <mergeCell ref="H30:J31"/>
-    <mergeCell ref="K30:M31"/>
-    <mergeCell ref="N30:P31"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:D39"/>
-    <mergeCell ref="E38:G39"/>
-    <mergeCell ref="H38:J39"/>
-    <mergeCell ref="K38:M39"/>
-    <mergeCell ref="N38:P39"/>
-    <mergeCell ref="Q34:S35"/>
-    <mergeCell ref="T34:T35"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:D37"/>
-    <mergeCell ref="E36:G37"/>
-    <mergeCell ref="H36:J37"/>
-    <mergeCell ref="K36:M37"/>
-    <mergeCell ref="N36:P37"/>
-    <mergeCell ref="Q38:S39"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:D35"/>
-    <mergeCell ref="E34:G35"/>
-    <mergeCell ref="H34:J35"/>
-    <mergeCell ref="K34:M35"/>
-    <mergeCell ref="N34:P35"/>
-    <mergeCell ref="AI39:AI40"/>
-    <mergeCell ref="AI41:AI42"/>
-    <mergeCell ref="AI43:AI44"/>
-    <mergeCell ref="Q36:S37"/>
-    <mergeCell ref="T36:T37"/>
-    <mergeCell ref="U36:U37"/>
-    <mergeCell ref="AI37:AI38"/>
-    <mergeCell ref="AI35:AI36"/>
-    <mergeCell ref="AI54:AI55"/>
-    <mergeCell ref="AI56:AI57"/>
-    <mergeCell ref="AI58:AI59"/>
-    <mergeCell ref="AI60:AI61"/>
-    <mergeCell ref="AC46:AE46"/>
-    <mergeCell ref="AF46:AH46"/>
-    <mergeCell ref="AI46:AI47"/>
-    <mergeCell ref="AI48:AI49"/>
-    <mergeCell ref="AI50:AI51"/>
-    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AC12:AE12"/>
+    <mergeCell ref="AF12:AH12"/>
+    <mergeCell ref="AI12:AK12"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:S23"/>
   </mergeCells>
   <conditionalFormatting sqref="AB14:AL27">
     <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
@@ -17871,20 +17832,20 @@
       <c r="N2" s="6">
         <v>30</v>
       </c>
-      <c r="O2" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="200" t="s">
+      <c r="O2" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="205" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="201"/>
-      <c r="R2" s="202"/>
-      <c r="S2" s="200" t="s">
+      <c r="Q2" s="206"/>
+      <c r="R2" s="207"/>
+      <c r="S2" s="205" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="201"/>
-      <c r="U2" s="202"/>
-      <c r="V2" s="203" t="s">
+      <c r="T2" s="206"/>
+      <c r="U2" s="207"/>
+      <c r="V2" s="199" t="s">
         <v>14</v>
       </c>
     </row>
@@ -17946,7 +17907,7 @@
       <c r="U3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="204"/>
+      <c r="V3" s="200"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
@@ -18653,7 +18614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
@@ -19173,25 +19134,25 @@
       <c r="P9" s="172"/>
       <c r="Q9" s="172"/>
       <c r="R9" s="172"/>
-      <c r="U9" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="V9" s="207" t="s">
+      <c r="U9" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="195" t="s">
         <v>18</v>
       </c>
-      <c r="W9" s="208"/>
-      <c r="X9" s="209"/>
-      <c r="Y9" s="207" t="s">
+      <c r="W9" s="196"/>
+      <c r="X9" s="197"/>
+      <c r="Y9" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="Z9" s="208"/>
-      <c r="AA9" s="209"/>
-      <c r="AB9" s="207" t="s">
+      <c r="Z9" s="196"/>
+      <c r="AA9" s="197"/>
+      <c r="AB9" s="195" t="s">
         <v>114</v>
       </c>
-      <c r="AC9" s="208"/>
-      <c r="AD9" s="210"/>
-      <c r="AE9" s="203" t="s">
+      <c r="AC9" s="196"/>
+      <c r="AD9" s="198"/>
+      <c r="AE9" s="199" t="s">
         <v>14</v>
       </c>
     </row>
@@ -19234,7 +19195,7 @@
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
-      <c r="U10" s="204"/>
+      <c r="U10" s="200"/>
       <c r="V10" s="40" t="s">
         <v>26</v>
       </c>
@@ -19262,7 +19223,7 @@
       <c r="AD10" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="AE10" s="204"/>
+      <c r="AE10" s="200"/>
     </row>
     <row r="11" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -19312,10 +19273,10 @@
       <c r="Q11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R11" s="215" t="s">
+      <c r="R11" s="216" t="s">
         <v>150</v>
       </c>
-      <c r="S11" s="193"/>
+      <c r="S11" s="212"/>
       <c r="U11" s="44" t="s">
         <v>7</v>
       </c>
@@ -19346,7 +19307,7 @@
       <c r="AD11" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AE11" s="211">
+      <c r="AE11" s="201">
         <f>SUM(Z11:Z12,AC11:AC12,W11:W12)</f>
         <v>26</v>
       </c>
@@ -19410,7 +19371,7 @@
       <c r="AB12" s="50"/>
       <c r="AC12" s="51"/>
       <c r="AD12" s="24"/>
-      <c r="AE12" s="199"/>
+      <c r="AE12" s="193"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
@@ -19487,7 +19448,7 @@
       <c r="AD13" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="AE13" s="199">
+      <c r="AE13" s="193">
         <f t="shared" ref="AE13" si="7">SUM(Z13:Z14,AC13:AC14,W13:W14)</f>
         <v>27</v>
       </c>
@@ -19557,7 +19518,7 @@
       <c r="AB14" s="45"/>
       <c r="AC14" s="46"/>
       <c r="AD14" s="8"/>
-      <c r="AE14" s="199"/>
+      <c r="AE14" s="193"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
@@ -19638,7 +19599,7 @@
       <c r="AD15" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="AE15" s="199">
+      <c r="AE15" s="193">
         <f t="shared" ref="AE15" si="8">SUM(Z15:Z16,AC15:AC16,W15:W16)</f>
         <v>26</v>
       </c>
@@ -19714,7 +19675,7 @@
       <c r="AD16" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="AE16" s="199"/>
+      <c r="AE16" s="193"/>
     </row>
     <row r="17" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
@@ -19795,7 +19756,7 @@
       <c r="AD17" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AE17" s="199">
+      <c r="AE17" s="193">
         <f t="shared" ref="AE17" si="9">SUM(Z17:Z18,AC17:AC18,W17:W18)</f>
         <v>28</v>
       </c>
@@ -19861,7 +19822,7 @@
       <c r="AD18" s="69" t="s">
         <v>135</v>
       </c>
-      <c r="AE18" s="199"/>
+      <c r="AE18" s="193"/>
     </row>
     <row r="19" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="U19" s="53" t="s">
@@ -19894,7 +19855,7 @@
       <c r="AD19" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="AE19" s="199">
+      <c r="AE19" s="193">
         <f t="shared" ref="AE19" si="10">SUM(Z19:Z20,AC19:AC20,W19:W20)</f>
         <v>30</v>
       </c>
@@ -19941,7 +19902,7 @@
         <v>2</v>
       </c>
       <c r="AD20" s="24"/>
-      <c r="AE20" s="199"/>
+      <c r="AE20" s="193"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="U21" s="44" t="s">
@@ -19974,7 +19935,7 @@
       <c r="AD21" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="AE21" s="199">
+      <c r="AE21" s="193">
         <f t="shared" ref="AE21" si="11">SUM(Z21:Z22,AC21:AC22,W21:W22)</f>
         <v>28</v>
       </c>
@@ -19991,7 +19952,7 @@
       <c r="AB22" s="45"/>
       <c r="AC22" s="46"/>
       <c r="AD22" s="8"/>
-      <c r="AE22" s="199"/>
+      <c r="AE22" s="193"/>
     </row>
     <row r="23" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="U23" s="53" t="s">
@@ -20024,7 +19985,7 @@
       <c r="AD23" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="AE23" s="199">
+      <c r="AE23" s="193">
         <f t="shared" ref="AE23" si="12">SUM(Z23:Z24,AC23:AC24,W23:W24)</f>
         <v>28</v>
       </c>
@@ -20091,7 +20052,7 @@
       <c r="AD24" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="AE24" s="213"/>
+      <c r="AE24" s="194"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
@@ -20314,17 +20275,17 @@
       <c r="R28" s="6">
         <v>15</v>
       </c>
-      <c r="U28" s="216"/>
-      <c r="V28" s="216"/>
-      <c r="W28" s="216"/>
-      <c r="X28" s="216"/>
-      <c r="Y28" s="216"/>
-      <c r="Z28" s="216"/>
-      <c r="AA28" s="216"/>
-      <c r="AB28" s="216"/>
-      <c r="AC28" s="216"/>
-      <c r="AD28" s="216"/>
-      <c r="AE28" s="216"/>
+      <c r="U28" s="215"/>
+      <c r="V28" s="215"/>
+      <c r="W28" s="215"/>
+      <c r="X28" s="215"/>
+      <c r="Y28" s="215"/>
+      <c r="Z28" s="215"/>
+      <c r="AA28" s="215"/>
+      <c r="AB28" s="215"/>
+      <c r="AC28" s="215"/>
+      <c r="AD28" s="215"/>
+      <c r="AE28" s="215"/>
     </row>
     <row r="29" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -20373,7 +20334,7 @@
       <c r="R29" s="6">
         <v>22</v>
       </c>
-      <c r="U29" s="216"/>
+      <c r="U29" s="215"/>
       <c r="V29" s="73"/>
       <c r="W29" s="73"/>
       <c r="X29" s="73"/>
@@ -20383,7 +20344,7 @@
       <c r="AB29" s="73"/>
       <c r="AC29" s="73"/>
       <c r="AD29" s="73"/>
-      <c r="AE29" s="216"/>
+      <c r="AE29" s="215"/>
     </row>
     <row r="30" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
@@ -20446,7 +20407,7 @@
       <c r="AB30" s="73"/>
       <c r="AC30" s="73"/>
       <c r="AD30" s="73"/>
-      <c r="AE30" s="216"/>
+      <c r="AE30" s="215"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
@@ -20498,7 +20459,7 @@
       <c r="AB31" s="73"/>
       <c r="AC31" s="73"/>
       <c r="AD31" s="73"/>
-      <c r="AE31" s="216"/>
+      <c r="AE31" s="215"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
@@ -20548,7 +20509,7 @@
       <c r="AB32" s="73"/>
       <c r="AC32" s="73"/>
       <c r="AD32" s="73"/>
-      <c r="AE32" s="216"/>
+      <c r="AE32" s="215"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
@@ -20594,7 +20555,7 @@
       <c r="AB33" s="73"/>
       <c r="AC33" s="73"/>
       <c r="AD33" s="73"/>
-      <c r="AE33" s="216"/>
+      <c r="AE33" s="215"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
@@ -20644,7 +20605,7 @@
       <c r="AB34" s="73"/>
       <c r="AC34" s="73"/>
       <c r="AD34" s="73"/>
-      <c r="AE34" s="216"/>
+      <c r="AE34" s="215"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
@@ -20694,7 +20655,7 @@
       <c r="AB35" s="73"/>
       <c r="AC35" s="73"/>
       <c r="AD35" s="73"/>
-      <c r="AE35" s="216"/>
+      <c r="AE35" s="215"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
@@ -20740,7 +20701,7 @@
       <c r="AB36" s="73"/>
       <c r="AC36" s="73"/>
       <c r="AD36" s="73"/>
-      <c r="AE36" s="216"/>
+      <c r="AE36" s="215"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
@@ -20790,7 +20751,7 @@
       <c r="AB37" s="73"/>
       <c r="AC37" s="73"/>
       <c r="AD37" s="181"/>
-      <c r="AE37" s="216"/>
+      <c r="AE37" s="215"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
@@ -20840,7 +20801,7 @@
       <c r="AB38" s="73"/>
       <c r="AC38" s="73"/>
       <c r="AD38" s="73"/>
-      <c r="AE38" s="216"/>
+      <c r="AE38" s="215"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" s="59" t="s">
@@ -20890,7 +20851,7 @@
       <c r="AB39" s="73"/>
       <c r="AC39" s="73"/>
       <c r="AD39" s="73"/>
-      <c r="AE39" s="216"/>
+      <c r="AE39" s="215"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
@@ -20940,7 +20901,7 @@
       <c r="AB40" s="73"/>
       <c r="AC40" s="73"/>
       <c r="AD40" s="73"/>
-      <c r="AE40" s="216"/>
+      <c r="AE40" s="215"/>
     </row>
     <row r="41" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="62"/>
@@ -20986,7 +20947,7 @@
       <c r="AB41" s="73"/>
       <c r="AC41" s="73"/>
       <c r="AD41" s="73"/>
-      <c r="AE41" s="216"/>
+      <c r="AE41" s="215"/>
     </row>
     <row r="42" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="U42" s="73"/>
@@ -20999,7 +20960,7 @@
       <c r="AB42" s="73"/>
       <c r="AC42" s="73"/>
       <c r="AD42" s="73"/>
-      <c r="AE42" s="216"/>
+      <c r="AE42" s="215"/>
     </row>
     <row r="43" spans="1:31" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="70" t="s">
@@ -21029,7 +20990,7 @@
       <c r="AB43" s="73"/>
       <c r="AC43" s="73"/>
       <c r="AD43" s="73"/>
-      <c r="AE43" s="216"/>
+      <c r="AE43" s="215"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="U44" s="73"/>
@@ -21046,18 +21007,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="AE40:AE41"/>
-    <mergeCell ref="AE42:AE43"/>
-    <mergeCell ref="AE30:AE31"/>
-    <mergeCell ref="AE32:AE33"/>
-    <mergeCell ref="AE34:AE35"/>
-    <mergeCell ref="AE36:AE37"/>
-    <mergeCell ref="AE38:AE39"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="V28:X28"/>
-    <mergeCell ref="Y28:AA28"/>
-    <mergeCell ref="AB28:AD28"/>
-    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Y9:AA9"/>
     <mergeCell ref="AE21:AE22"/>
     <mergeCell ref="AE23:AE24"/>
     <mergeCell ref="AE9:AE10"/>
@@ -21066,11 +21020,18 @@
     <mergeCell ref="AE15:AE16"/>
     <mergeCell ref="AE17:AE18"/>
     <mergeCell ref="AE19:AE20"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="V28:X28"/>
+    <mergeCell ref="Y28:AA28"/>
+    <mergeCell ref="AB28:AD28"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AE40:AE41"/>
+    <mergeCell ref="AE42:AE43"/>
+    <mergeCell ref="AE30:AE31"/>
+    <mergeCell ref="AE32:AE33"/>
+    <mergeCell ref="AE34:AE35"/>
+    <mergeCell ref="AE36:AE37"/>
+    <mergeCell ref="AE38:AE39"/>
   </mergeCells>
   <conditionalFormatting sqref="Z26">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="notEqual">
@@ -21114,7 +21075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E29" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Y54" sqref="Y54"/>
     </sheetView>
   </sheetViews>
@@ -21459,20 +21420,20 @@
       <c r="R6" s="6">
         <v>15</v>
       </c>
-      <c r="T6" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="207" t="s">
+      <c r="T6" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="195" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="208"/>
-      <c r="W6" s="209"/>
-      <c r="X6" s="207" t="s">
+      <c r="V6" s="196"/>
+      <c r="W6" s="197"/>
+      <c r="X6" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" s="208"/>
-      <c r="Z6" s="210"/>
-      <c r="AA6" s="203" t="s">
+      <c r="Y6" s="196"/>
+      <c r="Z6" s="198"/>
+      <c r="AA6" s="199" t="s">
         <v>14</v>
       </c>
     </row>
@@ -21526,7 +21487,7 @@
         <f>SUM(Q2:Q6)</f>
         <v>6992</v>
       </c>
-      <c r="T7" s="204"/>
+      <c r="T7" s="200"/>
       <c r="U7" s="40" t="s">
         <v>26</v>
       </c>
@@ -21545,7 +21506,7 @@
       <c r="Z7" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="AA7" s="204"/>
+      <c r="AA7" s="200"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -21609,7 +21570,7 @@
       <c r="Z8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AA8" s="211">
+      <c r="AA8" s="201">
         <f>SUM(V8:V9,Y8:Y9)</f>
         <v>52</v>
       </c>
@@ -21662,7 +21623,7 @@
       <c r="Z9" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AA9" s="199"/>
+      <c r="AA9" s="193"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
@@ -21724,7 +21685,7 @@
       <c r="Z10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AA10" s="199">
+      <c r="AA10" s="193">
         <f t="shared" ref="AA10" si="7">SUM(V10:V11,Y10:Y11)</f>
         <v>52</v>
       </c>
@@ -21787,7 +21748,7 @@
       <c r="Z11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AA11" s="199"/>
+      <c r="AA11" s="193"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
@@ -21848,7 +21809,7 @@
       <c r="Z12" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="AA12" s="199">
+      <c r="AA12" s="193">
         <f t="shared" ref="AA12" si="8">SUM(V12:V13,Y12:Y13)</f>
         <v>52</v>
       </c>
@@ -21916,7 +21877,7 @@
       <c r="Z13" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AA13" s="199"/>
+      <c r="AA13" s="193"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
@@ -21981,7 +21942,7 @@
       <c r="Z14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AA14" s="199">
+      <c r="AA14" s="193">
         <f t="shared" ref="AA14" si="9">SUM(V14:V15,Y14:Y15)</f>
         <v>57</v>
       </c>
@@ -22043,7 +22004,7 @@
       <c r="Z15" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="AA15" s="199"/>
+      <c r="AA15" s="193"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
@@ -22110,7 +22071,7 @@
       <c r="Z16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AA16" s="199">
+      <c r="AA16" s="193">
         <f t="shared" ref="AA16" si="10">SUM(V16:V17,Y16:Y17)</f>
         <v>54</v>
       </c>
@@ -22176,7 +22137,7 @@
       <c r="Z17" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="AA17" s="199"/>
+      <c r="AA17" s="193"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
@@ -22237,7 +22198,7 @@
       <c r="Z18" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="AA18" s="199">
+      <c r="AA18" s="193">
         <f t="shared" ref="AA18" si="11">SUM(V18:V19,Y18:Y19)</f>
         <v>54</v>
       </c>
@@ -22305,7 +22266,7 @@
       <c r="Z19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AA19" s="199"/>
+      <c r="AA19" s="193"/>
     </row>
     <row r="20" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
@@ -22366,7 +22327,7 @@
       <c r="Z20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="AA20" s="199">
+      <c r="AA20" s="193">
         <f t="shared" ref="AA20" si="12">SUM(V20:V21,Y20:Y21)</f>
         <v>52</v>
       </c>
@@ -22428,7 +22389,7 @@
       <c r="Z21" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="AA21" s="213"/>
+      <c r="AA21" s="194"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
@@ -22743,6 +22704,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="AA20:AA21"/>
     <mergeCell ref="O12:O13"/>
     <mergeCell ref="P12:Q12"/>
@@ -22750,12 +22717,6 @@
     <mergeCell ref="AA14:AA15"/>
     <mergeCell ref="AA16:AA17"/>
     <mergeCell ref="AA18:AA19"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AA8:AA9"/>
   </mergeCells>
   <conditionalFormatting sqref="Y24">
     <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
@@ -22969,20 +22930,20 @@
       <c r="R3" s="6">
         <v>20</v>
       </c>
-      <c r="T3" s="203" t="s">
-        <v>0</v>
-      </c>
-      <c r="U3" s="207" t="s">
+      <c r="T3" s="199" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="195" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="208"/>
-      <c r="W3" s="209"/>
-      <c r="X3" s="207" t="s">
+      <c r="V3" s="196"/>
+      <c r="W3" s="197"/>
+      <c r="X3" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="Y3" s="208"/>
-      <c r="Z3" s="210"/>
-      <c r="AA3" s="203" t="s">
+      <c r="Y3" s="196"/>
+      <c r="Z3" s="198"/>
+      <c r="AA3" s="199" t="s">
         <v>14</v>
       </c>
     </row>
@@ -23034,7 +22995,7 @@
       <c r="R4" s="6">
         <v>15</v>
       </c>
-      <c r="T4" s="204"/>
+      <c r="T4" s="200"/>
       <c r="U4" s="40" t="s">
         <v>26</v>
       </c>
@@ -23053,7 +23014,7 @@
       <c r="Z4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="204"/>
+      <c r="AA4" s="200"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="96" t="s">
@@ -23128,7 +23089,7 @@
       <c r="Z5" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="AA5" s="211">
+      <c r="AA5" s="201">
         <f>SUM(V5:V6,Y5:Y6)</f>
         <v>18</v>
       </c>
@@ -23198,7 +23159,7 @@
       <c r="X6" s="131"/>
       <c r="Y6" s="51"/>
       <c r="Z6" s="133"/>
-      <c r="AA6" s="199"/>
+      <c r="AA6" s="193"/>
     </row>
     <row r="7" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
@@ -23266,7 +23227,7 @@
       <c r="Z7" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="AA7" s="199">
+      <c r="AA7" s="193">
         <f t="shared" ref="AA7" si="7">SUM(V7:V8,Y7:Y8)</f>
         <v>18</v>
       </c>
@@ -23322,7 +23283,7 @@
       <c r="Z8" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="AA8" s="199"/>
+      <c r="AA8" s="193"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
@@ -23383,7 +23344,7 @@
       <c r="Z9" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AA9" s="199">
+      <c r="AA9" s="193">
         <f t="shared" ref="AA9" si="8">SUM(V9:V10,Y9:Y10)</f>
         <v>18</v>
       </c>
@@ -23429,7 +23390,7 @@
       <c r="X10" s="131"/>
       <c r="Y10" s="51"/>
       <c r="Z10" s="133"/>
-      <c r="AA10" s="199"/>
+      <c r="AA10" s="193"/>
     </row>
     <row r="11" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -23464,7 +23425,7 @@
       <c r="Z11" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AA11" s="199">
+      <c r="AA11" s="193">
         <f t="shared" ref="AA11" si="9">SUM(V11:V12,Y11:Y12)</f>
         <v>18</v>
       </c>
@@ -23507,9 +23468,9 @@
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="O12" s="207"/>
-      <c r="P12" s="208"/>
-      <c r="Q12" s="209"/>
+      <c r="O12" s="195"/>
+      <c r="P12" s="196"/>
+      <c r="Q12" s="197"/>
       <c r="T12" s="44"/>
       <c r="U12" s="130"/>
       <c r="V12" s="46"/>
@@ -23517,7 +23478,7 @@
       <c r="X12" s="130"/>
       <c r="Y12" s="46"/>
       <c r="Z12" s="73"/>
-      <c r="AA12" s="199"/>
+      <c r="AA12" s="193"/>
     </row>
     <row r="13" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
@@ -23550,7 +23511,7 @@
       <c r="Z13" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AA13" s="199">
+      <c r="AA13" s="193">
         <f t="shared" ref="AA13" si="12">SUM(V13:V14,Y13:Y14)</f>
         <v>18</v>
       </c>
@@ -23572,7 +23533,7 @@
       <c r="X14" s="131"/>
       <c r="Y14" s="51"/>
       <c r="Z14" s="133"/>
-      <c r="AA14" s="199"/>
+      <c r="AA14" s="193"/>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="109"/>
@@ -23605,7 +23566,7 @@
       <c r="Z15" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="AA15" s="199">
+      <c r="AA15" s="193">
         <f t="shared" ref="AA15" si="13">SUM(V15:V16,Y15:Y16)</f>
         <v>18</v>
       </c>
@@ -23627,7 +23588,7 @@
       <c r="X16" s="130"/>
       <c r="Y16" s="46"/>
       <c r="Z16" s="73"/>
-      <c r="AA16" s="199"/>
+      <c r="AA16" s="193"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
@@ -23660,7 +23621,7 @@
       <c r="Z17" s="58" t="s">
         <v>68</v>
       </c>
-      <c r="AA17" s="199">
+      <c r="AA17" s="193">
         <f t="shared" ref="AA17" si="14">SUM(V17:V18,Y17:Y18)</f>
         <v>16</v>
       </c>
@@ -23682,7 +23643,7 @@
       <c r="X18" s="136"/>
       <c r="Y18" s="77"/>
       <c r="Z18" s="138"/>
-      <c r="AA18" s="213"/>
+      <c r="AA18" s="194"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
@@ -23839,6 +23800,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AA5:AA6"/>
     <mergeCell ref="AA17:AA18"/>
     <mergeCell ref="AA9:AA10"/>
     <mergeCell ref="AA11:AA12"/>
@@ -23846,12 +23813,6 @@
     <mergeCell ref="P12:Q12"/>
     <mergeCell ref="AA13:AA14"/>
     <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AA5:AA6"/>
   </mergeCells>
   <conditionalFormatting sqref="Y20">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">

</xml_diff>